<commit_message>
feat: fixed excel data
</commit_message>
<xml_diff>
--- a/data/Alutech W62,W72.xlsx
+++ b/data/Alutech W62,W72.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48182092-E124-4796-9A7D-CA8841129D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD25CEE-E45B-4993-9333-1F5040830F9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="982" firstSheet="11" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="982" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Alutech до 2400 белый" sheetId="8" r:id="rId1"/>
@@ -1877,7 +1877,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="163">
+  <cellXfs count="162">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -2308,7 +2308,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -16223,9 +16222,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -16263,9 +16262,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -16298,26 +16297,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -16350,26 +16332,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -16549,12 +16514,12 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="32.44140625" customWidth="1"/>
-    <col min="2" max="2" width="67.44140625" customWidth="1"/>
-    <col min="3" max="3" width="22.77734375" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="32.453125" customWidth="1"/>
+    <col min="2" max="2" width="67.453125" customWidth="1"/>
+    <col min="3" max="3" width="22.81640625" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:5">
@@ -20115,11 +20080,11 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" customWidth="1"/>
-    <col min="2" max="2" width="68.88671875" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="27.36328125" customWidth="1"/>
+    <col min="2" max="2" width="68.90625" customWidth="1"/>
+    <col min="3" max="3" width="20.6328125" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
   </cols>
   <sheetData>
@@ -23777,11 +23742,11 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" customWidth="1"/>
-    <col min="2" max="2" width="69.44140625" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" customWidth="1"/>
+    <col min="1" max="1" width="21.6328125" customWidth="1"/>
+    <col min="2" max="2" width="69.453125" customWidth="1"/>
+    <col min="3" max="3" width="22.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:6">
@@ -23796,7 +23761,7 @@
       <c r="B6" t="s">
         <v>421</v>
       </c>
-      <c r="E6" s="162" t="s">
+      <c r="E6" t="s">
         <v>151</v>
       </c>
       <c r="F6" t="s">
@@ -27439,12 +27404,12 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="31.77734375" customWidth="1"/>
-    <col min="2" max="2" width="68.44140625" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="31.81640625" customWidth="1"/>
+    <col min="2" max="2" width="68.453125" customWidth="1"/>
+    <col min="3" max="3" width="23.08984375" customWidth="1"/>
+    <col min="5" max="5" width="12.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:6">
@@ -31244,12 +31209,12 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="22.21875" customWidth="1"/>
-    <col min="2" max="2" width="67.44140625" customWidth="1"/>
-    <col min="3" max="3" width="22.77734375" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="22.1796875" customWidth="1"/>
+    <col min="2" max="2" width="67.453125" customWidth="1"/>
+    <col min="3" max="3" width="22.81640625" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:6">
@@ -34957,11 +34922,11 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="27.44140625" customWidth="1"/>
-    <col min="2" max="2" width="68.88671875" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="27.453125" customWidth="1"/>
+    <col min="2" max="2" width="68.90625" customWidth="1"/>
+    <col min="3" max="3" width="20.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:6">
@@ -38618,11 +38583,11 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="69.44140625" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" customWidth="1"/>
+    <col min="2" max="2" width="69.453125" customWidth="1"/>
+    <col min="3" max="3" width="22.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:6">
@@ -42275,16 +42240,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A5:J393"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" customWidth="1"/>
-    <col min="2" max="2" width="68.44140625" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="27.36328125" customWidth="1"/>
+    <col min="2" max="2" width="68.453125" customWidth="1"/>
+    <col min="3" max="3" width="23.08984375" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:6">
@@ -46091,392 +46056,392 @@
       <selection pane="topRight" activeCell="B8" sqref="B8:B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.109375" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="14.08984375" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="24.44140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="24.453125" style="2" customWidth="1"/>
     <col min="2" max="2" width="36" style="2" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="23.6328125" style="2" customWidth="1"/>
     <col min="4" max="4" width="16" style="2" customWidth="1"/>
-    <col min="5" max="5" width="83.88671875" style="2" customWidth="1"/>
-    <col min="6" max="256" width="14.109375" style="2"/>
-    <col min="257" max="257" width="24.44140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="83.90625" style="2" customWidth="1"/>
+    <col min="6" max="256" width="14.08984375" style="2"/>
+    <col min="257" max="257" width="24.453125" style="2" customWidth="1"/>
     <col min="258" max="258" width="36" style="2" customWidth="1"/>
-    <col min="259" max="259" width="23.6640625" style="2" customWidth="1"/>
+    <col min="259" max="259" width="23.6328125" style="2" customWidth="1"/>
     <col min="260" max="260" width="16" style="2" customWidth="1"/>
-    <col min="261" max="261" width="83.88671875" style="2" customWidth="1"/>
-    <col min="262" max="512" width="14.109375" style="2"/>
-    <col min="513" max="513" width="24.44140625" style="2" customWidth="1"/>
+    <col min="261" max="261" width="83.90625" style="2" customWidth="1"/>
+    <col min="262" max="512" width="14.08984375" style="2"/>
+    <col min="513" max="513" width="24.453125" style="2" customWidth="1"/>
     <col min="514" max="514" width="36" style="2" customWidth="1"/>
-    <col min="515" max="515" width="23.6640625" style="2" customWidth="1"/>
+    <col min="515" max="515" width="23.6328125" style="2" customWidth="1"/>
     <col min="516" max="516" width="16" style="2" customWidth="1"/>
-    <col min="517" max="517" width="83.88671875" style="2" customWidth="1"/>
-    <col min="518" max="768" width="14.109375" style="2"/>
-    <col min="769" max="769" width="24.44140625" style="2" customWidth="1"/>
+    <col min="517" max="517" width="83.90625" style="2" customWidth="1"/>
+    <col min="518" max="768" width="14.08984375" style="2"/>
+    <col min="769" max="769" width="24.453125" style="2" customWidth="1"/>
     <col min="770" max="770" width="36" style="2" customWidth="1"/>
-    <col min="771" max="771" width="23.6640625" style="2" customWidth="1"/>
+    <col min="771" max="771" width="23.6328125" style="2" customWidth="1"/>
     <col min="772" max="772" width="16" style="2" customWidth="1"/>
-    <col min="773" max="773" width="83.88671875" style="2" customWidth="1"/>
-    <col min="774" max="1024" width="14.109375" style="2"/>
-    <col min="1025" max="1025" width="24.44140625" style="2" customWidth="1"/>
+    <col min="773" max="773" width="83.90625" style="2" customWidth="1"/>
+    <col min="774" max="1024" width="14.08984375" style="2"/>
+    <col min="1025" max="1025" width="24.453125" style="2" customWidth="1"/>
     <col min="1026" max="1026" width="36" style="2" customWidth="1"/>
-    <col min="1027" max="1027" width="23.6640625" style="2" customWidth="1"/>
+    <col min="1027" max="1027" width="23.6328125" style="2" customWidth="1"/>
     <col min="1028" max="1028" width="16" style="2" customWidth="1"/>
-    <col min="1029" max="1029" width="83.88671875" style="2" customWidth="1"/>
-    <col min="1030" max="1280" width="14.109375" style="2"/>
-    <col min="1281" max="1281" width="24.44140625" style="2" customWidth="1"/>
+    <col min="1029" max="1029" width="83.90625" style="2" customWidth="1"/>
+    <col min="1030" max="1280" width="14.08984375" style="2"/>
+    <col min="1281" max="1281" width="24.453125" style="2" customWidth="1"/>
     <col min="1282" max="1282" width="36" style="2" customWidth="1"/>
-    <col min="1283" max="1283" width="23.6640625" style="2" customWidth="1"/>
+    <col min="1283" max="1283" width="23.6328125" style="2" customWidth="1"/>
     <col min="1284" max="1284" width="16" style="2" customWidth="1"/>
-    <col min="1285" max="1285" width="83.88671875" style="2" customWidth="1"/>
-    <col min="1286" max="1536" width="14.109375" style="2"/>
-    <col min="1537" max="1537" width="24.44140625" style="2" customWidth="1"/>
+    <col min="1285" max="1285" width="83.90625" style="2" customWidth="1"/>
+    <col min="1286" max="1536" width="14.08984375" style="2"/>
+    <col min="1537" max="1537" width="24.453125" style="2" customWidth="1"/>
     <col min="1538" max="1538" width="36" style="2" customWidth="1"/>
-    <col min="1539" max="1539" width="23.6640625" style="2" customWidth="1"/>
+    <col min="1539" max="1539" width="23.6328125" style="2" customWidth="1"/>
     <col min="1540" max="1540" width="16" style="2" customWidth="1"/>
-    <col min="1541" max="1541" width="83.88671875" style="2" customWidth="1"/>
-    <col min="1542" max="1792" width="14.109375" style="2"/>
-    <col min="1793" max="1793" width="24.44140625" style="2" customWidth="1"/>
+    <col min="1541" max="1541" width="83.90625" style="2" customWidth="1"/>
+    <col min="1542" max="1792" width="14.08984375" style="2"/>
+    <col min="1793" max="1793" width="24.453125" style="2" customWidth="1"/>
     <col min="1794" max="1794" width="36" style="2" customWidth="1"/>
-    <col min="1795" max="1795" width="23.6640625" style="2" customWidth="1"/>
+    <col min="1795" max="1795" width="23.6328125" style="2" customWidth="1"/>
     <col min="1796" max="1796" width="16" style="2" customWidth="1"/>
-    <col min="1797" max="1797" width="83.88671875" style="2" customWidth="1"/>
-    <col min="1798" max="2048" width="14.109375" style="2"/>
-    <col min="2049" max="2049" width="24.44140625" style="2" customWidth="1"/>
+    <col min="1797" max="1797" width="83.90625" style="2" customWidth="1"/>
+    <col min="1798" max="2048" width="14.08984375" style="2"/>
+    <col min="2049" max="2049" width="24.453125" style="2" customWidth="1"/>
     <col min="2050" max="2050" width="36" style="2" customWidth="1"/>
-    <col min="2051" max="2051" width="23.6640625" style="2" customWidth="1"/>
+    <col min="2051" max="2051" width="23.6328125" style="2" customWidth="1"/>
     <col min="2052" max="2052" width="16" style="2" customWidth="1"/>
-    <col min="2053" max="2053" width="83.88671875" style="2" customWidth="1"/>
-    <col min="2054" max="2304" width="14.109375" style="2"/>
-    <col min="2305" max="2305" width="24.44140625" style="2" customWidth="1"/>
+    <col min="2053" max="2053" width="83.90625" style="2" customWidth="1"/>
+    <col min="2054" max="2304" width="14.08984375" style="2"/>
+    <col min="2305" max="2305" width="24.453125" style="2" customWidth="1"/>
     <col min="2306" max="2306" width="36" style="2" customWidth="1"/>
-    <col min="2307" max="2307" width="23.6640625" style="2" customWidth="1"/>
+    <col min="2307" max="2307" width="23.6328125" style="2" customWidth="1"/>
     <col min="2308" max="2308" width="16" style="2" customWidth="1"/>
-    <col min="2309" max="2309" width="83.88671875" style="2" customWidth="1"/>
-    <col min="2310" max="2560" width="14.109375" style="2"/>
-    <col min="2561" max="2561" width="24.44140625" style="2" customWidth="1"/>
+    <col min="2309" max="2309" width="83.90625" style="2" customWidth="1"/>
+    <col min="2310" max="2560" width="14.08984375" style="2"/>
+    <col min="2561" max="2561" width="24.453125" style="2" customWidth="1"/>
     <col min="2562" max="2562" width="36" style="2" customWidth="1"/>
-    <col min="2563" max="2563" width="23.6640625" style="2" customWidth="1"/>
+    <col min="2563" max="2563" width="23.6328125" style="2" customWidth="1"/>
     <col min="2564" max="2564" width="16" style="2" customWidth="1"/>
-    <col min="2565" max="2565" width="83.88671875" style="2" customWidth="1"/>
-    <col min="2566" max="2816" width="14.109375" style="2"/>
-    <col min="2817" max="2817" width="24.44140625" style="2" customWidth="1"/>
+    <col min="2565" max="2565" width="83.90625" style="2" customWidth="1"/>
+    <col min="2566" max="2816" width="14.08984375" style="2"/>
+    <col min="2817" max="2817" width="24.453125" style="2" customWidth="1"/>
     <col min="2818" max="2818" width="36" style="2" customWidth="1"/>
-    <col min="2819" max="2819" width="23.6640625" style="2" customWidth="1"/>
+    <col min="2819" max="2819" width="23.6328125" style="2" customWidth="1"/>
     <col min="2820" max="2820" width="16" style="2" customWidth="1"/>
-    <col min="2821" max="2821" width="83.88671875" style="2" customWidth="1"/>
-    <col min="2822" max="3072" width="14.109375" style="2"/>
-    <col min="3073" max="3073" width="24.44140625" style="2" customWidth="1"/>
+    <col min="2821" max="2821" width="83.90625" style="2" customWidth="1"/>
+    <col min="2822" max="3072" width="14.08984375" style="2"/>
+    <col min="3073" max="3073" width="24.453125" style="2" customWidth="1"/>
     <col min="3074" max="3074" width="36" style="2" customWidth="1"/>
-    <col min="3075" max="3075" width="23.6640625" style="2" customWidth="1"/>
+    <col min="3075" max="3075" width="23.6328125" style="2" customWidth="1"/>
     <col min="3076" max="3076" width="16" style="2" customWidth="1"/>
-    <col min="3077" max="3077" width="83.88671875" style="2" customWidth="1"/>
-    <col min="3078" max="3328" width="14.109375" style="2"/>
-    <col min="3329" max="3329" width="24.44140625" style="2" customWidth="1"/>
+    <col min="3077" max="3077" width="83.90625" style="2" customWidth="1"/>
+    <col min="3078" max="3328" width="14.08984375" style="2"/>
+    <col min="3329" max="3329" width="24.453125" style="2" customWidth="1"/>
     <col min="3330" max="3330" width="36" style="2" customWidth="1"/>
-    <col min="3331" max="3331" width="23.6640625" style="2" customWidth="1"/>
+    <col min="3331" max="3331" width="23.6328125" style="2" customWidth="1"/>
     <col min="3332" max="3332" width="16" style="2" customWidth="1"/>
-    <col min="3333" max="3333" width="83.88671875" style="2" customWidth="1"/>
-    <col min="3334" max="3584" width="14.109375" style="2"/>
-    <col min="3585" max="3585" width="24.44140625" style="2" customWidth="1"/>
+    <col min="3333" max="3333" width="83.90625" style="2" customWidth="1"/>
+    <col min="3334" max="3584" width="14.08984375" style="2"/>
+    <col min="3585" max="3585" width="24.453125" style="2" customWidth="1"/>
     <col min="3586" max="3586" width="36" style="2" customWidth="1"/>
-    <col min="3587" max="3587" width="23.6640625" style="2" customWidth="1"/>
+    <col min="3587" max="3587" width="23.6328125" style="2" customWidth="1"/>
     <col min="3588" max="3588" width="16" style="2" customWidth="1"/>
-    <col min="3589" max="3589" width="83.88671875" style="2" customWidth="1"/>
-    <col min="3590" max="3840" width="14.109375" style="2"/>
-    <col min="3841" max="3841" width="24.44140625" style="2" customWidth="1"/>
+    <col min="3589" max="3589" width="83.90625" style="2" customWidth="1"/>
+    <col min="3590" max="3840" width="14.08984375" style="2"/>
+    <col min="3841" max="3841" width="24.453125" style="2" customWidth="1"/>
     <col min="3842" max="3842" width="36" style="2" customWidth="1"/>
-    <col min="3843" max="3843" width="23.6640625" style="2" customWidth="1"/>
+    <col min="3843" max="3843" width="23.6328125" style="2" customWidth="1"/>
     <col min="3844" max="3844" width="16" style="2" customWidth="1"/>
-    <col min="3845" max="3845" width="83.88671875" style="2" customWidth="1"/>
-    <col min="3846" max="4096" width="14.109375" style="2"/>
-    <col min="4097" max="4097" width="24.44140625" style="2" customWidth="1"/>
+    <col min="3845" max="3845" width="83.90625" style="2" customWidth="1"/>
+    <col min="3846" max="4096" width="14.08984375" style="2"/>
+    <col min="4097" max="4097" width="24.453125" style="2" customWidth="1"/>
     <col min="4098" max="4098" width="36" style="2" customWidth="1"/>
-    <col min="4099" max="4099" width="23.6640625" style="2" customWidth="1"/>
+    <col min="4099" max="4099" width="23.6328125" style="2" customWidth="1"/>
     <col min="4100" max="4100" width="16" style="2" customWidth="1"/>
-    <col min="4101" max="4101" width="83.88671875" style="2" customWidth="1"/>
-    <col min="4102" max="4352" width="14.109375" style="2"/>
-    <col min="4353" max="4353" width="24.44140625" style="2" customWidth="1"/>
+    <col min="4101" max="4101" width="83.90625" style="2" customWidth="1"/>
+    <col min="4102" max="4352" width="14.08984375" style="2"/>
+    <col min="4353" max="4353" width="24.453125" style="2" customWidth="1"/>
     <col min="4354" max="4354" width="36" style="2" customWidth="1"/>
-    <col min="4355" max="4355" width="23.6640625" style="2" customWidth="1"/>
+    <col min="4355" max="4355" width="23.6328125" style="2" customWidth="1"/>
     <col min="4356" max="4356" width="16" style="2" customWidth="1"/>
-    <col min="4357" max="4357" width="83.88671875" style="2" customWidth="1"/>
-    <col min="4358" max="4608" width="14.109375" style="2"/>
-    <col min="4609" max="4609" width="24.44140625" style="2" customWidth="1"/>
+    <col min="4357" max="4357" width="83.90625" style="2" customWidth="1"/>
+    <col min="4358" max="4608" width="14.08984375" style="2"/>
+    <col min="4609" max="4609" width="24.453125" style="2" customWidth="1"/>
     <col min="4610" max="4610" width="36" style="2" customWidth="1"/>
-    <col min="4611" max="4611" width="23.6640625" style="2" customWidth="1"/>
+    <col min="4611" max="4611" width="23.6328125" style="2" customWidth="1"/>
     <col min="4612" max="4612" width="16" style="2" customWidth="1"/>
-    <col min="4613" max="4613" width="83.88671875" style="2" customWidth="1"/>
-    <col min="4614" max="4864" width="14.109375" style="2"/>
-    <col min="4865" max="4865" width="24.44140625" style="2" customWidth="1"/>
+    <col min="4613" max="4613" width="83.90625" style="2" customWidth="1"/>
+    <col min="4614" max="4864" width="14.08984375" style="2"/>
+    <col min="4865" max="4865" width="24.453125" style="2" customWidth="1"/>
     <col min="4866" max="4866" width="36" style="2" customWidth="1"/>
-    <col min="4867" max="4867" width="23.6640625" style="2" customWidth="1"/>
+    <col min="4867" max="4867" width="23.6328125" style="2" customWidth="1"/>
     <col min="4868" max="4868" width="16" style="2" customWidth="1"/>
-    <col min="4869" max="4869" width="83.88671875" style="2" customWidth="1"/>
-    <col min="4870" max="5120" width="14.109375" style="2"/>
-    <col min="5121" max="5121" width="24.44140625" style="2" customWidth="1"/>
+    <col min="4869" max="4869" width="83.90625" style="2" customWidth="1"/>
+    <col min="4870" max="5120" width="14.08984375" style="2"/>
+    <col min="5121" max="5121" width="24.453125" style="2" customWidth="1"/>
     <col min="5122" max="5122" width="36" style="2" customWidth="1"/>
-    <col min="5123" max="5123" width="23.6640625" style="2" customWidth="1"/>
+    <col min="5123" max="5123" width="23.6328125" style="2" customWidth="1"/>
     <col min="5124" max="5124" width="16" style="2" customWidth="1"/>
-    <col min="5125" max="5125" width="83.88671875" style="2" customWidth="1"/>
-    <col min="5126" max="5376" width="14.109375" style="2"/>
-    <col min="5377" max="5377" width="24.44140625" style="2" customWidth="1"/>
+    <col min="5125" max="5125" width="83.90625" style="2" customWidth="1"/>
+    <col min="5126" max="5376" width="14.08984375" style="2"/>
+    <col min="5377" max="5377" width="24.453125" style="2" customWidth="1"/>
     <col min="5378" max="5378" width="36" style="2" customWidth="1"/>
-    <col min="5379" max="5379" width="23.6640625" style="2" customWidth="1"/>
+    <col min="5379" max="5379" width="23.6328125" style="2" customWidth="1"/>
     <col min="5380" max="5380" width="16" style="2" customWidth="1"/>
-    <col min="5381" max="5381" width="83.88671875" style="2" customWidth="1"/>
-    <col min="5382" max="5632" width="14.109375" style="2"/>
-    <col min="5633" max="5633" width="24.44140625" style="2" customWidth="1"/>
+    <col min="5381" max="5381" width="83.90625" style="2" customWidth="1"/>
+    <col min="5382" max="5632" width="14.08984375" style="2"/>
+    <col min="5633" max="5633" width="24.453125" style="2" customWidth="1"/>
     <col min="5634" max="5634" width="36" style="2" customWidth="1"/>
-    <col min="5635" max="5635" width="23.6640625" style="2" customWidth="1"/>
+    <col min="5635" max="5635" width="23.6328125" style="2" customWidth="1"/>
     <col min="5636" max="5636" width="16" style="2" customWidth="1"/>
-    <col min="5637" max="5637" width="83.88671875" style="2" customWidth="1"/>
-    <col min="5638" max="5888" width="14.109375" style="2"/>
-    <col min="5889" max="5889" width="24.44140625" style="2" customWidth="1"/>
+    <col min="5637" max="5637" width="83.90625" style="2" customWidth="1"/>
+    <col min="5638" max="5888" width="14.08984375" style="2"/>
+    <col min="5889" max="5889" width="24.453125" style="2" customWidth="1"/>
     <col min="5890" max="5890" width="36" style="2" customWidth="1"/>
-    <col min="5891" max="5891" width="23.6640625" style="2" customWidth="1"/>
+    <col min="5891" max="5891" width="23.6328125" style="2" customWidth="1"/>
     <col min="5892" max="5892" width="16" style="2" customWidth="1"/>
-    <col min="5893" max="5893" width="83.88671875" style="2" customWidth="1"/>
-    <col min="5894" max="6144" width="14.109375" style="2"/>
-    <col min="6145" max="6145" width="24.44140625" style="2" customWidth="1"/>
+    <col min="5893" max="5893" width="83.90625" style="2" customWidth="1"/>
+    <col min="5894" max="6144" width="14.08984375" style="2"/>
+    <col min="6145" max="6145" width="24.453125" style="2" customWidth="1"/>
     <col min="6146" max="6146" width="36" style="2" customWidth="1"/>
-    <col min="6147" max="6147" width="23.6640625" style="2" customWidth="1"/>
+    <col min="6147" max="6147" width="23.6328125" style="2" customWidth="1"/>
     <col min="6148" max="6148" width="16" style="2" customWidth="1"/>
-    <col min="6149" max="6149" width="83.88671875" style="2" customWidth="1"/>
-    <col min="6150" max="6400" width="14.109375" style="2"/>
-    <col min="6401" max="6401" width="24.44140625" style="2" customWidth="1"/>
+    <col min="6149" max="6149" width="83.90625" style="2" customWidth="1"/>
+    <col min="6150" max="6400" width="14.08984375" style="2"/>
+    <col min="6401" max="6401" width="24.453125" style="2" customWidth="1"/>
     <col min="6402" max="6402" width="36" style="2" customWidth="1"/>
-    <col min="6403" max="6403" width="23.6640625" style="2" customWidth="1"/>
+    <col min="6403" max="6403" width="23.6328125" style="2" customWidth="1"/>
     <col min="6404" max="6404" width="16" style="2" customWidth="1"/>
-    <col min="6405" max="6405" width="83.88671875" style="2" customWidth="1"/>
-    <col min="6406" max="6656" width="14.109375" style="2"/>
-    <col min="6657" max="6657" width="24.44140625" style="2" customWidth="1"/>
+    <col min="6405" max="6405" width="83.90625" style="2" customWidth="1"/>
+    <col min="6406" max="6656" width="14.08984375" style="2"/>
+    <col min="6657" max="6657" width="24.453125" style="2" customWidth="1"/>
     <col min="6658" max="6658" width="36" style="2" customWidth="1"/>
-    <col min="6659" max="6659" width="23.6640625" style="2" customWidth="1"/>
+    <col min="6659" max="6659" width="23.6328125" style="2" customWidth="1"/>
     <col min="6660" max="6660" width="16" style="2" customWidth="1"/>
-    <col min="6661" max="6661" width="83.88671875" style="2" customWidth="1"/>
-    <col min="6662" max="6912" width="14.109375" style="2"/>
-    <col min="6913" max="6913" width="24.44140625" style="2" customWidth="1"/>
+    <col min="6661" max="6661" width="83.90625" style="2" customWidth="1"/>
+    <col min="6662" max="6912" width="14.08984375" style="2"/>
+    <col min="6913" max="6913" width="24.453125" style="2" customWidth="1"/>
     <col min="6914" max="6914" width="36" style="2" customWidth="1"/>
-    <col min="6915" max="6915" width="23.6640625" style="2" customWidth="1"/>
+    <col min="6915" max="6915" width="23.6328125" style="2" customWidth="1"/>
     <col min="6916" max="6916" width="16" style="2" customWidth="1"/>
-    <col min="6917" max="6917" width="83.88671875" style="2" customWidth="1"/>
-    <col min="6918" max="7168" width="14.109375" style="2"/>
-    <col min="7169" max="7169" width="24.44140625" style="2" customWidth="1"/>
+    <col min="6917" max="6917" width="83.90625" style="2" customWidth="1"/>
+    <col min="6918" max="7168" width="14.08984375" style="2"/>
+    <col min="7169" max="7169" width="24.453125" style="2" customWidth="1"/>
     <col min="7170" max="7170" width="36" style="2" customWidth="1"/>
-    <col min="7171" max="7171" width="23.6640625" style="2" customWidth="1"/>
+    <col min="7171" max="7171" width="23.6328125" style="2" customWidth="1"/>
     <col min="7172" max="7172" width="16" style="2" customWidth="1"/>
-    <col min="7173" max="7173" width="83.88671875" style="2" customWidth="1"/>
-    <col min="7174" max="7424" width="14.109375" style="2"/>
-    <col min="7425" max="7425" width="24.44140625" style="2" customWidth="1"/>
+    <col min="7173" max="7173" width="83.90625" style="2" customWidth="1"/>
+    <col min="7174" max="7424" width="14.08984375" style="2"/>
+    <col min="7425" max="7425" width="24.453125" style="2" customWidth="1"/>
     <col min="7426" max="7426" width="36" style="2" customWidth="1"/>
-    <col min="7427" max="7427" width="23.6640625" style="2" customWidth="1"/>
+    <col min="7427" max="7427" width="23.6328125" style="2" customWidth="1"/>
     <col min="7428" max="7428" width="16" style="2" customWidth="1"/>
-    <col min="7429" max="7429" width="83.88671875" style="2" customWidth="1"/>
-    <col min="7430" max="7680" width="14.109375" style="2"/>
-    <col min="7681" max="7681" width="24.44140625" style="2" customWidth="1"/>
+    <col min="7429" max="7429" width="83.90625" style="2" customWidth="1"/>
+    <col min="7430" max="7680" width="14.08984375" style="2"/>
+    <col min="7681" max="7681" width="24.453125" style="2" customWidth="1"/>
     <col min="7682" max="7682" width="36" style="2" customWidth="1"/>
-    <col min="7683" max="7683" width="23.6640625" style="2" customWidth="1"/>
+    <col min="7683" max="7683" width="23.6328125" style="2" customWidth="1"/>
     <col min="7684" max="7684" width="16" style="2" customWidth="1"/>
-    <col min="7685" max="7685" width="83.88671875" style="2" customWidth="1"/>
-    <col min="7686" max="7936" width="14.109375" style="2"/>
-    <col min="7937" max="7937" width="24.44140625" style="2" customWidth="1"/>
+    <col min="7685" max="7685" width="83.90625" style="2" customWidth="1"/>
+    <col min="7686" max="7936" width="14.08984375" style="2"/>
+    <col min="7937" max="7937" width="24.453125" style="2" customWidth="1"/>
     <col min="7938" max="7938" width="36" style="2" customWidth="1"/>
-    <col min="7939" max="7939" width="23.6640625" style="2" customWidth="1"/>
+    <col min="7939" max="7939" width="23.6328125" style="2" customWidth="1"/>
     <col min="7940" max="7940" width="16" style="2" customWidth="1"/>
-    <col min="7941" max="7941" width="83.88671875" style="2" customWidth="1"/>
-    <col min="7942" max="8192" width="14.109375" style="2"/>
-    <col min="8193" max="8193" width="24.44140625" style="2" customWidth="1"/>
+    <col min="7941" max="7941" width="83.90625" style="2" customWidth="1"/>
+    <col min="7942" max="8192" width="14.08984375" style="2"/>
+    <col min="8193" max="8193" width="24.453125" style="2" customWidth="1"/>
     <col min="8194" max="8194" width="36" style="2" customWidth="1"/>
-    <col min="8195" max="8195" width="23.6640625" style="2" customWidth="1"/>
+    <col min="8195" max="8195" width="23.6328125" style="2" customWidth="1"/>
     <col min="8196" max="8196" width="16" style="2" customWidth="1"/>
-    <col min="8197" max="8197" width="83.88671875" style="2" customWidth="1"/>
-    <col min="8198" max="8448" width="14.109375" style="2"/>
-    <col min="8449" max="8449" width="24.44140625" style="2" customWidth="1"/>
+    <col min="8197" max="8197" width="83.90625" style="2" customWidth="1"/>
+    <col min="8198" max="8448" width="14.08984375" style="2"/>
+    <col min="8449" max="8449" width="24.453125" style="2" customWidth="1"/>
     <col min="8450" max="8450" width="36" style="2" customWidth="1"/>
-    <col min="8451" max="8451" width="23.6640625" style="2" customWidth="1"/>
+    <col min="8451" max="8451" width="23.6328125" style="2" customWidth="1"/>
     <col min="8452" max="8452" width="16" style="2" customWidth="1"/>
-    <col min="8453" max="8453" width="83.88671875" style="2" customWidth="1"/>
-    <col min="8454" max="8704" width="14.109375" style="2"/>
-    <col min="8705" max="8705" width="24.44140625" style="2" customWidth="1"/>
+    <col min="8453" max="8453" width="83.90625" style="2" customWidth="1"/>
+    <col min="8454" max="8704" width="14.08984375" style="2"/>
+    <col min="8705" max="8705" width="24.453125" style="2" customWidth="1"/>
     <col min="8706" max="8706" width="36" style="2" customWidth="1"/>
-    <col min="8707" max="8707" width="23.6640625" style="2" customWidth="1"/>
+    <col min="8707" max="8707" width="23.6328125" style="2" customWidth="1"/>
     <col min="8708" max="8708" width="16" style="2" customWidth="1"/>
-    <col min="8709" max="8709" width="83.88671875" style="2" customWidth="1"/>
-    <col min="8710" max="8960" width="14.109375" style="2"/>
-    <col min="8961" max="8961" width="24.44140625" style="2" customWidth="1"/>
+    <col min="8709" max="8709" width="83.90625" style="2" customWidth="1"/>
+    <col min="8710" max="8960" width="14.08984375" style="2"/>
+    <col min="8961" max="8961" width="24.453125" style="2" customWidth="1"/>
     <col min="8962" max="8962" width="36" style="2" customWidth="1"/>
-    <col min="8963" max="8963" width="23.6640625" style="2" customWidth="1"/>
+    <col min="8963" max="8963" width="23.6328125" style="2" customWidth="1"/>
     <col min="8964" max="8964" width="16" style="2" customWidth="1"/>
-    <col min="8965" max="8965" width="83.88671875" style="2" customWidth="1"/>
-    <col min="8966" max="9216" width="14.109375" style="2"/>
-    <col min="9217" max="9217" width="24.44140625" style="2" customWidth="1"/>
+    <col min="8965" max="8965" width="83.90625" style="2" customWidth="1"/>
+    <col min="8966" max="9216" width="14.08984375" style="2"/>
+    <col min="9217" max="9217" width="24.453125" style="2" customWidth="1"/>
     <col min="9218" max="9218" width="36" style="2" customWidth="1"/>
-    <col min="9219" max="9219" width="23.6640625" style="2" customWidth="1"/>
+    <col min="9219" max="9219" width="23.6328125" style="2" customWidth="1"/>
     <col min="9220" max="9220" width="16" style="2" customWidth="1"/>
-    <col min="9221" max="9221" width="83.88671875" style="2" customWidth="1"/>
-    <col min="9222" max="9472" width="14.109375" style="2"/>
-    <col min="9473" max="9473" width="24.44140625" style="2" customWidth="1"/>
+    <col min="9221" max="9221" width="83.90625" style="2" customWidth="1"/>
+    <col min="9222" max="9472" width="14.08984375" style="2"/>
+    <col min="9473" max="9473" width="24.453125" style="2" customWidth="1"/>
     <col min="9474" max="9474" width="36" style="2" customWidth="1"/>
-    <col min="9475" max="9475" width="23.6640625" style="2" customWidth="1"/>
+    <col min="9475" max="9475" width="23.6328125" style="2" customWidth="1"/>
     <col min="9476" max="9476" width="16" style="2" customWidth="1"/>
-    <col min="9477" max="9477" width="83.88671875" style="2" customWidth="1"/>
-    <col min="9478" max="9728" width="14.109375" style="2"/>
-    <col min="9729" max="9729" width="24.44140625" style="2" customWidth="1"/>
+    <col min="9477" max="9477" width="83.90625" style="2" customWidth="1"/>
+    <col min="9478" max="9728" width="14.08984375" style="2"/>
+    <col min="9729" max="9729" width="24.453125" style="2" customWidth="1"/>
     <col min="9730" max="9730" width="36" style="2" customWidth="1"/>
-    <col min="9731" max="9731" width="23.6640625" style="2" customWidth="1"/>
+    <col min="9731" max="9731" width="23.6328125" style="2" customWidth="1"/>
     <col min="9732" max="9732" width="16" style="2" customWidth="1"/>
-    <col min="9733" max="9733" width="83.88671875" style="2" customWidth="1"/>
-    <col min="9734" max="9984" width="14.109375" style="2"/>
-    <col min="9985" max="9985" width="24.44140625" style="2" customWidth="1"/>
+    <col min="9733" max="9733" width="83.90625" style="2" customWidth="1"/>
+    <col min="9734" max="9984" width="14.08984375" style="2"/>
+    <col min="9985" max="9985" width="24.453125" style="2" customWidth="1"/>
     <col min="9986" max="9986" width="36" style="2" customWidth="1"/>
-    <col min="9987" max="9987" width="23.6640625" style="2" customWidth="1"/>
+    <col min="9987" max="9987" width="23.6328125" style="2" customWidth="1"/>
     <col min="9988" max="9988" width="16" style="2" customWidth="1"/>
-    <col min="9989" max="9989" width="83.88671875" style="2" customWidth="1"/>
-    <col min="9990" max="10240" width="14.109375" style="2"/>
-    <col min="10241" max="10241" width="24.44140625" style="2" customWidth="1"/>
+    <col min="9989" max="9989" width="83.90625" style="2" customWidth="1"/>
+    <col min="9990" max="10240" width="14.08984375" style="2"/>
+    <col min="10241" max="10241" width="24.453125" style="2" customWidth="1"/>
     <col min="10242" max="10242" width="36" style="2" customWidth="1"/>
-    <col min="10243" max="10243" width="23.6640625" style="2" customWidth="1"/>
+    <col min="10243" max="10243" width="23.6328125" style="2" customWidth="1"/>
     <col min="10244" max="10244" width="16" style="2" customWidth="1"/>
-    <col min="10245" max="10245" width="83.88671875" style="2" customWidth="1"/>
-    <col min="10246" max="10496" width="14.109375" style="2"/>
-    <col min="10497" max="10497" width="24.44140625" style="2" customWidth="1"/>
+    <col min="10245" max="10245" width="83.90625" style="2" customWidth="1"/>
+    <col min="10246" max="10496" width="14.08984375" style="2"/>
+    <col min="10497" max="10497" width="24.453125" style="2" customWidth="1"/>
     <col min="10498" max="10498" width="36" style="2" customWidth="1"/>
-    <col min="10499" max="10499" width="23.6640625" style="2" customWidth="1"/>
+    <col min="10499" max="10499" width="23.6328125" style="2" customWidth="1"/>
     <col min="10500" max="10500" width="16" style="2" customWidth="1"/>
-    <col min="10501" max="10501" width="83.88671875" style="2" customWidth="1"/>
-    <col min="10502" max="10752" width="14.109375" style="2"/>
-    <col min="10753" max="10753" width="24.44140625" style="2" customWidth="1"/>
+    <col min="10501" max="10501" width="83.90625" style="2" customWidth="1"/>
+    <col min="10502" max="10752" width="14.08984375" style="2"/>
+    <col min="10753" max="10753" width="24.453125" style="2" customWidth="1"/>
     <col min="10754" max="10754" width="36" style="2" customWidth="1"/>
-    <col min="10755" max="10755" width="23.6640625" style="2" customWidth="1"/>
+    <col min="10755" max="10755" width="23.6328125" style="2" customWidth="1"/>
     <col min="10756" max="10756" width="16" style="2" customWidth="1"/>
-    <col min="10757" max="10757" width="83.88671875" style="2" customWidth="1"/>
-    <col min="10758" max="11008" width="14.109375" style="2"/>
-    <col min="11009" max="11009" width="24.44140625" style="2" customWidth="1"/>
+    <col min="10757" max="10757" width="83.90625" style="2" customWidth="1"/>
+    <col min="10758" max="11008" width="14.08984375" style="2"/>
+    <col min="11009" max="11009" width="24.453125" style="2" customWidth="1"/>
     <col min="11010" max="11010" width="36" style="2" customWidth="1"/>
-    <col min="11011" max="11011" width="23.6640625" style="2" customWidth="1"/>
+    <col min="11011" max="11011" width="23.6328125" style="2" customWidth="1"/>
     <col min="11012" max="11012" width="16" style="2" customWidth="1"/>
-    <col min="11013" max="11013" width="83.88671875" style="2" customWidth="1"/>
-    <col min="11014" max="11264" width="14.109375" style="2"/>
-    <col min="11265" max="11265" width="24.44140625" style="2" customWidth="1"/>
+    <col min="11013" max="11013" width="83.90625" style="2" customWidth="1"/>
+    <col min="11014" max="11264" width="14.08984375" style="2"/>
+    <col min="11265" max="11265" width="24.453125" style="2" customWidth="1"/>
     <col min="11266" max="11266" width="36" style="2" customWidth="1"/>
-    <col min="11267" max="11267" width="23.6640625" style="2" customWidth="1"/>
+    <col min="11267" max="11267" width="23.6328125" style="2" customWidth="1"/>
     <col min="11268" max="11268" width="16" style="2" customWidth="1"/>
-    <col min="11269" max="11269" width="83.88671875" style="2" customWidth="1"/>
-    <col min="11270" max="11520" width="14.109375" style="2"/>
-    <col min="11521" max="11521" width="24.44140625" style="2" customWidth="1"/>
+    <col min="11269" max="11269" width="83.90625" style="2" customWidth="1"/>
+    <col min="11270" max="11520" width="14.08984375" style="2"/>
+    <col min="11521" max="11521" width="24.453125" style="2" customWidth="1"/>
     <col min="11522" max="11522" width="36" style="2" customWidth="1"/>
-    <col min="11523" max="11523" width="23.6640625" style="2" customWidth="1"/>
+    <col min="11523" max="11523" width="23.6328125" style="2" customWidth="1"/>
     <col min="11524" max="11524" width="16" style="2" customWidth="1"/>
-    <col min="11525" max="11525" width="83.88671875" style="2" customWidth="1"/>
-    <col min="11526" max="11776" width="14.109375" style="2"/>
-    <col min="11777" max="11777" width="24.44140625" style="2" customWidth="1"/>
+    <col min="11525" max="11525" width="83.90625" style="2" customWidth="1"/>
+    <col min="11526" max="11776" width="14.08984375" style="2"/>
+    <col min="11777" max="11777" width="24.453125" style="2" customWidth="1"/>
     <col min="11778" max="11778" width="36" style="2" customWidth="1"/>
-    <col min="11779" max="11779" width="23.6640625" style="2" customWidth="1"/>
+    <col min="11779" max="11779" width="23.6328125" style="2" customWidth="1"/>
     <col min="11780" max="11780" width="16" style="2" customWidth="1"/>
-    <col min="11781" max="11781" width="83.88671875" style="2" customWidth="1"/>
-    <col min="11782" max="12032" width="14.109375" style="2"/>
-    <col min="12033" max="12033" width="24.44140625" style="2" customWidth="1"/>
+    <col min="11781" max="11781" width="83.90625" style="2" customWidth="1"/>
+    <col min="11782" max="12032" width="14.08984375" style="2"/>
+    <col min="12033" max="12033" width="24.453125" style="2" customWidth="1"/>
     <col min="12034" max="12034" width="36" style="2" customWidth="1"/>
-    <col min="12035" max="12035" width="23.6640625" style="2" customWidth="1"/>
+    <col min="12035" max="12035" width="23.6328125" style="2" customWidth="1"/>
     <col min="12036" max="12036" width="16" style="2" customWidth="1"/>
-    <col min="12037" max="12037" width="83.88671875" style="2" customWidth="1"/>
-    <col min="12038" max="12288" width="14.109375" style="2"/>
-    <col min="12289" max="12289" width="24.44140625" style="2" customWidth="1"/>
+    <col min="12037" max="12037" width="83.90625" style="2" customWidth="1"/>
+    <col min="12038" max="12288" width="14.08984375" style="2"/>
+    <col min="12289" max="12289" width="24.453125" style="2" customWidth="1"/>
     <col min="12290" max="12290" width="36" style="2" customWidth="1"/>
-    <col min="12291" max="12291" width="23.6640625" style="2" customWidth="1"/>
+    <col min="12291" max="12291" width="23.6328125" style="2" customWidth="1"/>
     <col min="12292" max="12292" width="16" style="2" customWidth="1"/>
-    <col min="12293" max="12293" width="83.88671875" style="2" customWidth="1"/>
-    <col min="12294" max="12544" width="14.109375" style="2"/>
-    <col min="12545" max="12545" width="24.44140625" style="2" customWidth="1"/>
+    <col min="12293" max="12293" width="83.90625" style="2" customWidth="1"/>
+    <col min="12294" max="12544" width="14.08984375" style="2"/>
+    <col min="12545" max="12545" width="24.453125" style="2" customWidth="1"/>
     <col min="12546" max="12546" width="36" style="2" customWidth="1"/>
-    <col min="12547" max="12547" width="23.6640625" style="2" customWidth="1"/>
+    <col min="12547" max="12547" width="23.6328125" style="2" customWidth="1"/>
     <col min="12548" max="12548" width="16" style="2" customWidth="1"/>
-    <col min="12549" max="12549" width="83.88671875" style="2" customWidth="1"/>
-    <col min="12550" max="12800" width="14.109375" style="2"/>
-    <col min="12801" max="12801" width="24.44140625" style="2" customWidth="1"/>
+    <col min="12549" max="12549" width="83.90625" style="2" customWidth="1"/>
+    <col min="12550" max="12800" width="14.08984375" style="2"/>
+    <col min="12801" max="12801" width="24.453125" style="2" customWidth="1"/>
     <col min="12802" max="12802" width="36" style="2" customWidth="1"/>
-    <col min="12803" max="12803" width="23.6640625" style="2" customWidth="1"/>
+    <col min="12803" max="12803" width="23.6328125" style="2" customWidth="1"/>
     <col min="12804" max="12804" width="16" style="2" customWidth="1"/>
-    <col min="12805" max="12805" width="83.88671875" style="2" customWidth="1"/>
-    <col min="12806" max="13056" width="14.109375" style="2"/>
-    <col min="13057" max="13057" width="24.44140625" style="2" customWidth="1"/>
+    <col min="12805" max="12805" width="83.90625" style="2" customWidth="1"/>
+    <col min="12806" max="13056" width="14.08984375" style="2"/>
+    <col min="13057" max="13057" width="24.453125" style="2" customWidth="1"/>
     <col min="13058" max="13058" width="36" style="2" customWidth="1"/>
-    <col min="13059" max="13059" width="23.6640625" style="2" customWidth="1"/>
+    <col min="13059" max="13059" width="23.6328125" style="2" customWidth="1"/>
     <col min="13060" max="13060" width="16" style="2" customWidth="1"/>
-    <col min="13061" max="13061" width="83.88671875" style="2" customWidth="1"/>
-    <col min="13062" max="13312" width="14.109375" style="2"/>
-    <col min="13313" max="13313" width="24.44140625" style="2" customWidth="1"/>
+    <col min="13061" max="13061" width="83.90625" style="2" customWidth="1"/>
+    <col min="13062" max="13312" width="14.08984375" style="2"/>
+    <col min="13313" max="13313" width="24.453125" style="2" customWidth="1"/>
     <col min="13314" max="13314" width="36" style="2" customWidth="1"/>
-    <col min="13315" max="13315" width="23.6640625" style="2" customWidth="1"/>
+    <col min="13315" max="13315" width="23.6328125" style="2" customWidth="1"/>
     <col min="13316" max="13316" width="16" style="2" customWidth="1"/>
-    <col min="13317" max="13317" width="83.88671875" style="2" customWidth="1"/>
-    <col min="13318" max="13568" width="14.109375" style="2"/>
-    <col min="13569" max="13569" width="24.44140625" style="2" customWidth="1"/>
+    <col min="13317" max="13317" width="83.90625" style="2" customWidth="1"/>
+    <col min="13318" max="13568" width="14.08984375" style="2"/>
+    <col min="13569" max="13569" width="24.453125" style="2" customWidth="1"/>
     <col min="13570" max="13570" width="36" style="2" customWidth="1"/>
-    <col min="13571" max="13571" width="23.6640625" style="2" customWidth="1"/>
+    <col min="13571" max="13571" width="23.6328125" style="2" customWidth="1"/>
     <col min="13572" max="13572" width="16" style="2" customWidth="1"/>
-    <col min="13573" max="13573" width="83.88671875" style="2" customWidth="1"/>
-    <col min="13574" max="13824" width="14.109375" style="2"/>
-    <col min="13825" max="13825" width="24.44140625" style="2" customWidth="1"/>
+    <col min="13573" max="13573" width="83.90625" style="2" customWidth="1"/>
+    <col min="13574" max="13824" width="14.08984375" style="2"/>
+    <col min="13825" max="13825" width="24.453125" style="2" customWidth="1"/>
     <col min="13826" max="13826" width="36" style="2" customWidth="1"/>
-    <col min="13827" max="13827" width="23.6640625" style="2" customWidth="1"/>
+    <col min="13827" max="13827" width="23.6328125" style="2" customWidth="1"/>
     <col min="13828" max="13828" width="16" style="2" customWidth="1"/>
-    <col min="13829" max="13829" width="83.88671875" style="2" customWidth="1"/>
-    <col min="13830" max="14080" width="14.109375" style="2"/>
-    <col min="14081" max="14081" width="24.44140625" style="2" customWidth="1"/>
+    <col min="13829" max="13829" width="83.90625" style="2" customWidth="1"/>
+    <col min="13830" max="14080" width="14.08984375" style="2"/>
+    <col min="14081" max="14081" width="24.453125" style="2" customWidth="1"/>
     <col min="14082" max="14082" width="36" style="2" customWidth="1"/>
-    <col min="14083" max="14083" width="23.6640625" style="2" customWidth="1"/>
+    <col min="14083" max="14083" width="23.6328125" style="2" customWidth="1"/>
     <col min="14084" max="14084" width="16" style="2" customWidth="1"/>
-    <col min="14085" max="14085" width="83.88671875" style="2" customWidth="1"/>
-    <col min="14086" max="14336" width="14.109375" style="2"/>
-    <col min="14337" max="14337" width="24.44140625" style="2" customWidth="1"/>
+    <col min="14085" max="14085" width="83.90625" style="2" customWidth="1"/>
+    <col min="14086" max="14336" width="14.08984375" style="2"/>
+    <col min="14337" max="14337" width="24.453125" style="2" customWidth="1"/>
     <col min="14338" max="14338" width="36" style="2" customWidth="1"/>
-    <col min="14339" max="14339" width="23.6640625" style="2" customWidth="1"/>
+    <col min="14339" max="14339" width="23.6328125" style="2" customWidth="1"/>
     <col min="14340" max="14340" width="16" style="2" customWidth="1"/>
-    <col min="14341" max="14341" width="83.88671875" style="2" customWidth="1"/>
-    <col min="14342" max="14592" width="14.109375" style="2"/>
-    <col min="14593" max="14593" width="24.44140625" style="2" customWidth="1"/>
+    <col min="14341" max="14341" width="83.90625" style="2" customWidth="1"/>
+    <col min="14342" max="14592" width="14.08984375" style="2"/>
+    <col min="14593" max="14593" width="24.453125" style="2" customWidth="1"/>
     <col min="14594" max="14594" width="36" style="2" customWidth="1"/>
-    <col min="14595" max="14595" width="23.6640625" style="2" customWidth="1"/>
+    <col min="14595" max="14595" width="23.6328125" style="2" customWidth="1"/>
     <col min="14596" max="14596" width="16" style="2" customWidth="1"/>
-    <col min="14597" max="14597" width="83.88671875" style="2" customWidth="1"/>
-    <col min="14598" max="14848" width="14.109375" style="2"/>
-    <col min="14849" max="14849" width="24.44140625" style="2" customWidth="1"/>
+    <col min="14597" max="14597" width="83.90625" style="2" customWidth="1"/>
+    <col min="14598" max="14848" width="14.08984375" style="2"/>
+    <col min="14849" max="14849" width="24.453125" style="2" customWidth="1"/>
     <col min="14850" max="14850" width="36" style="2" customWidth="1"/>
-    <col min="14851" max="14851" width="23.6640625" style="2" customWidth="1"/>
+    <col min="14851" max="14851" width="23.6328125" style="2" customWidth="1"/>
     <col min="14852" max="14852" width="16" style="2" customWidth="1"/>
-    <col min="14853" max="14853" width="83.88671875" style="2" customWidth="1"/>
-    <col min="14854" max="15104" width="14.109375" style="2"/>
-    <col min="15105" max="15105" width="24.44140625" style="2" customWidth="1"/>
+    <col min="14853" max="14853" width="83.90625" style="2" customWidth="1"/>
+    <col min="14854" max="15104" width="14.08984375" style="2"/>
+    <col min="15105" max="15105" width="24.453125" style="2" customWidth="1"/>
     <col min="15106" max="15106" width="36" style="2" customWidth="1"/>
-    <col min="15107" max="15107" width="23.6640625" style="2" customWidth="1"/>
+    <col min="15107" max="15107" width="23.6328125" style="2" customWidth="1"/>
     <col min="15108" max="15108" width="16" style="2" customWidth="1"/>
-    <col min="15109" max="15109" width="83.88671875" style="2" customWidth="1"/>
-    <col min="15110" max="15360" width="14.109375" style="2"/>
-    <col min="15361" max="15361" width="24.44140625" style="2" customWidth="1"/>
+    <col min="15109" max="15109" width="83.90625" style="2" customWidth="1"/>
+    <col min="15110" max="15360" width="14.08984375" style="2"/>
+    <col min="15361" max="15361" width="24.453125" style="2" customWidth="1"/>
     <col min="15362" max="15362" width="36" style="2" customWidth="1"/>
-    <col min="15363" max="15363" width="23.6640625" style="2" customWidth="1"/>
+    <col min="15363" max="15363" width="23.6328125" style="2" customWidth="1"/>
     <col min="15364" max="15364" width="16" style="2" customWidth="1"/>
-    <col min="15365" max="15365" width="83.88671875" style="2" customWidth="1"/>
-    <col min="15366" max="15616" width="14.109375" style="2"/>
-    <col min="15617" max="15617" width="24.44140625" style="2" customWidth="1"/>
+    <col min="15365" max="15365" width="83.90625" style="2" customWidth="1"/>
+    <col min="15366" max="15616" width="14.08984375" style="2"/>
+    <col min="15617" max="15617" width="24.453125" style="2" customWidth="1"/>
     <col min="15618" max="15618" width="36" style="2" customWidth="1"/>
-    <col min="15619" max="15619" width="23.6640625" style="2" customWidth="1"/>
+    <col min="15619" max="15619" width="23.6328125" style="2" customWidth="1"/>
     <col min="15620" max="15620" width="16" style="2" customWidth="1"/>
-    <col min="15621" max="15621" width="83.88671875" style="2" customWidth="1"/>
-    <col min="15622" max="15872" width="14.109375" style="2"/>
-    <col min="15873" max="15873" width="24.44140625" style="2" customWidth="1"/>
+    <col min="15621" max="15621" width="83.90625" style="2" customWidth="1"/>
+    <col min="15622" max="15872" width="14.08984375" style="2"/>
+    <col min="15873" max="15873" width="24.453125" style="2" customWidth="1"/>
     <col min="15874" max="15874" width="36" style="2" customWidth="1"/>
-    <col min="15875" max="15875" width="23.6640625" style="2" customWidth="1"/>
+    <col min="15875" max="15875" width="23.6328125" style="2" customWidth="1"/>
     <col min="15876" max="15876" width="16" style="2" customWidth="1"/>
-    <col min="15877" max="15877" width="83.88671875" style="2" customWidth="1"/>
-    <col min="15878" max="16128" width="14.109375" style="2"/>
-    <col min="16129" max="16129" width="24.44140625" style="2" customWidth="1"/>
+    <col min="15877" max="15877" width="83.90625" style="2" customWidth="1"/>
+    <col min="15878" max="16128" width="14.08984375" style="2"/>
+    <col min="16129" max="16129" width="24.453125" style="2" customWidth="1"/>
     <col min="16130" max="16130" width="36" style="2" customWidth="1"/>
-    <col min="16131" max="16131" width="23.6640625" style="2" customWidth="1"/>
+    <col min="16131" max="16131" width="23.6328125" style="2" customWidth="1"/>
     <col min="16132" max="16132" width="16" style="2" customWidth="1"/>
-    <col min="16133" max="16133" width="83.88671875" style="2" customWidth="1"/>
-    <col min="16134" max="16384" width="14.109375" style="2"/>
+    <col min="16133" max="16133" width="83.90625" style="2" customWidth="1"/>
+    <col min="16134" max="16384" width="14.08984375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="9" customHeight="1"/>
@@ -46730,7 +46695,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="14.4" thickBot="1">
+    <row r="22" spans="1:5" ht="14.5" thickBot="1">
       <c r="A22" s="94"/>
       <c r="B22" s="102"/>
       <c r="C22" s="14" t="s">
@@ -46749,13 +46714,13 @@
       <c r="D23" s="6"/>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="14.4" thickBot="1">
+    <row r="24" spans="1:5" ht="14.5" thickBot="1">
       <c r="A24" s="5"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5" ht="13.95" customHeight="1">
+    <row r="25" spans="1:5" ht="14" customHeight="1">
       <c r="A25" s="107" t="s">
         <v>78</v>
       </c>
@@ -46945,7 +46910,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="14.4" thickBot="1">
+    <row r="39" spans="1:5" ht="14.5" thickBot="1">
       <c r="A39" s="94"/>
       <c r="B39" s="102"/>
       <c r="C39" s="15">
@@ -46958,7 +46923,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="14.4" thickBot="1">
+    <row r="40" spans="1:5" ht="14.5" thickBot="1">
       <c r="A40" s="5"/>
       <c r="B40" s="17"/>
       <c r="C40" s="6"/>
@@ -46993,7 +46958,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="14.4" thickBot="1">
+    <row r="43" spans="1:5" ht="14.5" thickBot="1">
       <c r="A43" s="5"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
@@ -47040,7 +47005,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="14.4" thickBot="1">
+    <row r="47" spans="1:5" ht="14.5" thickBot="1">
       <c r="A47" s="104"/>
       <c r="B47" s="102"/>
       <c r="C47" s="14" t="s">
@@ -47053,13 +47018,13 @@
         <v>91</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="14.4" thickBot="1">
+    <row r="48" spans="1:5" ht="14.5" thickBot="1">
       <c r="A48" s="5"/>
       <c r="C48" s="6"/>
       <c r="D48" s="6"/>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:5" ht="57.6" customHeight="1" thickBot="1">
+    <row r="49" spans="1:5" ht="57.65" customHeight="1" thickBot="1">
       <c r="A49" s="25" t="s">
         <v>92</v>
       </c>
@@ -47223,7 +47188,7 @@
       <c r="D62" s="32"/>
       <c r="E62" s="95"/>
     </row>
-    <row r="63" spans="1:5" ht="13.95" customHeight="1">
+    <row r="63" spans="1:5" ht="14" customHeight="1">
       <c r="A63" s="93"/>
       <c r="B63" s="35" t="s">
         <v>109</v>
@@ -47245,7 +47210,7 @@
       <c r="D64" s="32"/>
       <c r="E64" s="95"/>
     </row>
-    <row r="65" spans="1:5" ht="14.4" thickBot="1">
+    <row r="65" spans="1:5" ht="14.5" thickBot="1">
       <c r="A65" s="94"/>
       <c r="B65" s="36" t="s">
         <v>111</v>
@@ -47269,7 +47234,7 @@
       <c r="D66" s="32"/>
       <c r="E66" s="95"/>
     </row>
-    <row r="67" spans="1:5" ht="13.95" customHeight="1">
+    <row r="67" spans="1:5" ht="14" customHeight="1">
       <c r="A67" s="93"/>
       <c r="B67" s="35" t="s">
         <v>97</v>
@@ -47315,7 +47280,7 @@
       <c r="D70" s="32"/>
       <c r="E70" s="95"/>
     </row>
-    <row r="71" spans="1:5" ht="13.95" customHeight="1">
+    <row r="71" spans="1:5" ht="14" customHeight="1">
       <c r="A71" s="93"/>
       <c r="B71" s="35" t="s">
         <v>101</v>
@@ -47361,7 +47326,7 @@
       <c r="D74" s="32"/>
       <c r="E74" s="95"/>
     </row>
-    <row r="75" spans="1:5" ht="13.95" customHeight="1">
+    <row r="75" spans="1:5" ht="14" customHeight="1">
       <c r="A75" s="93"/>
       <c r="B75" s="35" t="s">
         <v>105</v>
@@ -47407,7 +47372,7 @@
       <c r="D78" s="32"/>
       <c r="E78" s="95"/>
     </row>
-    <row r="79" spans="1:5" ht="13.95" customHeight="1">
+    <row r="79" spans="1:5" ht="14" customHeight="1">
       <c r="A79" s="93"/>
       <c r="B79" s="35" t="s">
         <v>109</v>
@@ -47429,7 +47394,7 @@
       <c r="D80" s="32"/>
       <c r="E80" s="95"/>
     </row>
-    <row r="81" spans="1:5" ht="14.4" thickBot="1">
+    <row r="81" spans="1:5" ht="14.5" thickBot="1">
       <c r="A81" s="94"/>
       <c r="B81" s="36" t="s">
         <v>124</v>
@@ -47453,7 +47418,7 @@
       <c r="D82" s="32"/>
       <c r="E82" s="95"/>
     </row>
-    <row r="83" spans="1:5" ht="13.95" customHeight="1">
+    <row r="83" spans="1:5" ht="14" customHeight="1">
       <c r="A83" s="93"/>
       <c r="B83" s="35" t="s">
         <v>97</v>
@@ -47499,7 +47464,7 @@
       <c r="D86" s="32"/>
       <c r="E86" s="95"/>
     </row>
-    <row r="87" spans="1:5" ht="13.95" customHeight="1">
+    <row r="87" spans="1:5" ht="14" customHeight="1">
       <c r="A87" s="93"/>
       <c r="B87" s="35" t="s">
         <v>101</v>
@@ -47545,7 +47510,7 @@
       <c r="D90" s="32"/>
       <c r="E90" s="95"/>
     </row>
-    <row r="91" spans="1:5" ht="13.95" customHeight="1">
+    <row r="91" spans="1:5" ht="14" customHeight="1">
       <c r="A91" s="93"/>
       <c r="B91" s="35" t="s">
         <v>105</v>
@@ -47567,7 +47532,7 @@
       <c r="D92" s="32"/>
       <c r="E92" s="96"/>
     </row>
-    <row r="93" spans="1:5" ht="14.4" thickBot="1">
+    <row r="93" spans="1:5" ht="14.5" thickBot="1">
       <c r="A93" s="94"/>
       <c r="B93" s="36" t="s">
         <v>134</v>
@@ -47591,7 +47556,7 @@
       <c r="D94" s="32"/>
       <c r="E94" s="95"/>
     </row>
-    <row r="95" spans="1:5" ht="13.95" customHeight="1">
+    <row r="95" spans="1:5" ht="14" customHeight="1">
       <c r="A95" s="93"/>
       <c r="B95" s="35" t="s">
         <v>97</v>
@@ -47637,7 +47602,7 @@
       <c r="D98" s="32"/>
       <c r="E98" s="95"/>
     </row>
-    <row r="99" spans="1:5" ht="13.95" customHeight="1">
+    <row r="99" spans="1:5" ht="14" customHeight="1">
       <c r="A99" s="93"/>
       <c r="B99" s="35" t="s">
         <v>101</v>
@@ -47683,7 +47648,7 @@
       <c r="D102" s="32"/>
       <c r="E102" s="95"/>
     </row>
-    <row r="103" spans="1:5" ht="13.95" customHeight="1">
+    <row r="103" spans="1:5" ht="14" customHeight="1">
       <c r="A103" s="93"/>
       <c r="B103" s="35" t="s">
         <v>105</v>
@@ -47729,7 +47694,7 @@
       <c r="D106" s="32"/>
       <c r="E106" s="95"/>
     </row>
-    <row r="107" spans="1:5" ht="13.95" customHeight="1">
+    <row r="107" spans="1:5" ht="14" customHeight="1">
       <c r="A107" s="93"/>
       <c r="B107" s="35" t="s">
         <v>109</v>
@@ -47751,7 +47716,7 @@
       <c r="D108" s="32"/>
       <c r="E108" s="95"/>
     </row>
-    <row r="109" spans="1:5" ht="14.4" thickBot="1">
+    <row r="109" spans="1:5" ht="14.5" thickBot="1">
       <c r="A109" s="94"/>
       <c r="B109" s="36" t="s">
         <v>147</v>
@@ -47834,402 +47799,402 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.77734375" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="14.81640625" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.6640625" style="40" customWidth="1"/>
-    <col min="3" max="3" width="26.77734375" style="40" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" style="40" customWidth="1"/>
-    <col min="5" max="5" width="87.44140625" style="40" customWidth="1"/>
-    <col min="6" max="256" width="14.77734375" style="40"/>
-    <col min="257" max="257" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="258" max="258" width="33.6640625" style="40" customWidth="1"/>
-    <col min="259" max="259" width="14.6640625" style="40" customWidth="1"/>
-    <col min="260" max="260" width="13.44140625" style="40" customWidth="1"/>
-    <col min="261" max="261" width="74.6640625" style="40" customWidth="1"/>
-    <col min="262" max="512" width="14.77734375" style="40"/>
-    <col min="513" max="513" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="514" max="514" width="33.6640625" style="40" customWidth="1"/>
-    <col min="515" max="515" width="14.6640625" style="40" customWidth="1"/>
-    <col min="516" max="516" width="13.44140625" style="40" customWidth="1"/>
-    <col min="517" max="517" width="74.6640625" style="40" customWidth="1"/>
-    <col min="518" max="768" width="14.77734375" style="40"/>
-    <col min="769" max="769" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="770" max="770" width="33.6640625" style="40" customWidth="1"/>
-    <col min="771" max="771" width="14.6640625" style="40" customWidth="1"/>
-    <col min="772" max="772" width="13.44140625" style="40" customWidth="1"/>
-    <col min="773" max="773" width="74.6640625" style="40" customWidth="1"/>
-    <col min="774" max="1024" width="14.77734375" style="40"/>
-    <col min="1025" max="1025" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="1026" max="1026" width="33.6640625" style="40" customWidth="1"/>
-    <col min="1027" max="1027" width="14.6640625" style="40" customWidth="1"/>
-    <col min="1028" max="1028" width="13.44140625" style="40" customWidth="1"/>
-    <col min="1029" max="1029" width="74.6640625" style="40" customWidth="1"/>
-    <col min="1030" max="1280" width="14.77734375" style="40"/>
-    <col min="1281" max="1281" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="1282" max="1282" width="33.6640625" style="40" customWidth="1"/>
-    <col min="1283" max="1283" width="14.6640625" style="40" customWidth="1"/>
-    <col min="1284" max="1284" width="13.44140625" style="40" customWidth="1"/>
-    <col min="1285" max="1285" width="74.6640625" style="40" customWidth="1"/>
-    <col min="1286" max="1536" width="14.77734375" style="40"/>
-    <col min="1537" max="1537" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="1538" max="1538" width="33.6640625" style="40" customWidth="1"/>
-    <col min="1539" max="1539" width="14.6640625" style="40" customWidth="1"/>
-    <col min="1540" max="1540" width="13.44140625" style="40" customWidth="1"/>
-    <col min="1541" max="1541" width="74.6640625" style="40" customWidth="1"/>
-    <col min="1542" max="1792" width="14.77734375" style="40"/>
-    <col min="1793" max="1793" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="1794" max="1794" width="33.6640625" style="40" customWidth="1"/>
-    <col min="1795" max="1795" width="14.6640625" style="40" customWidth="1"/>
-    <col min="1796" max="1796" width="13.44140625" style="40" customWidth="1"/>
-    <col min="1797" max="1797" width="74.6640625" style="40" customWidth="1"/>
-    <col min="1798" max="2048" width="14.77734375" style="40"/>
-    <col min="2049" max="2049" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="2050" max="2050" width="33.6640625" style="40" customWidth="1"/>
-    <col min="2051" max="2051" width="14.6640625" style="40" customWidth="1"/>
-    <col min="2052" max="2052" width="13.44140625" style="40" customWidth="1"/>
-    <col min="2053" max="2053" width="74.6640625" style="40" customWidth="1"/>
-    <col min="2054" max="2304" width="14.77734375" style="40"/>
-    <col min="2305" max="2305" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="2306" max="2306" width="33.6640625" style="40" customWidth="1"/>
-    <col min="2307" max="2307" width="14.6640625" style="40" customWidth="1"/>
-    <col min="2308" max="2308" width="13.44140625" style="40" customWidth="1"/>
-    <col min="2309" max="2309" width="74.6640625" style="40" customWidth="1"/>
-    <col min="2310" max="2560" width="14.77734375" style="40"/>
-    <col min="2561" max="2561" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="2562" max="2562" width="33.6640625" style="40" customWidth="1"/>
-    <col min="2563" max="2563" width="14.6640625" style="40" customWidth="1"/>
-    <col min="2564" max="2564" width="13.44140625" style="40" customWidth="1"/>
-    <col min="2565" max="2565" width="74.6640625" style="40" customWidth="1"/>
-    <col min="2566" max="2816" width="14.77734375" style="40"/>
-    <col min="2817" max="2817" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="2818" max="2818" width="33.6640625" style="40" customWidth="1"/>
-    <col min="2819" max="2819" width="14.6640625" style="40" customWidth="1"/>
-    <col min="2820" max="2820" width="13.44140625" style="40" customWidth="1"/>
-    <col min="2821" max="2821" width="74.6640625" style="40" customWidth="1"/>
-    <col min="2822" max="3072" width="14.77734375" style="40"/>
-    <col min="3073" max="3073" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="3074" max="3074" width="33.6640625" style="40" customWidth="1"/>
-    <col min="3075" max="3075" width="14.6640625" style="40" customWidth="1"/>
-    <col min="3076" max="3076" width="13.44140625" style="40" customWidth="1"/>
-    <col min="3077" max="3077" width="74.6640625" style="40" customWidth="1"/>
-    <col min="3078" max="3328" width="14.77734375" style="40"/>
-    <col min="3329" max="3329" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="3330" max="3330" width="33.6640625" style="40" customWidth="1"/>
-    <col min="3331" max="3331" width="14.6640625" style="40" customWidth="1"/>
-    <col min="3332" max="3332" width="13.44140625" style="40" customWidth="1"/>
-    <col min="3333" max="3333" width="74.6640625" style="40" customWidth="1"/>
-    <col min="3334" max="3584" width="14.77734375" style="40"/>
-    <col min="3585" max="3585" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="3586" max="3586" width="33.6640625" style="40" customWidth="1"/>
-    <col min="3587" max="3587" width="14.6640625" style="40" customWidth="1"/>
-    <col min="3588" max="3588" width="13.44140625" style="40" customWidth="1"/>
-    <col min="3589" max="3589" width="74.6640625" style="40" customWidth="1"/>
-    <col min="3590" max="3840" width="14.77734375" style="40"/>
-    <col min="3841" max="3841" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="3842" max="3842" width="33.6640625" style="40" customWidth="1"/>
-    <col min="3843" max="3843" width="14.6640625" style="40" customWidth="1"/>
-    <col min="3844" max="3844" width="13.44140625" style="40" customWidth="1"/>
-    <col min="3845" max="3845" width="74.6640625" style="40" customWidth="1"/>
-    <col min="3846" max="4096" width="14.77734375" style="40"/>
-    <col min="4097" max="4097" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="4098" max="4098" width="33.6640625" style="40" customWidth="1"/>
-    <col min="4099" max="4099" width="14.6640625" style="40" customWidth="1"/>
-    <col min="4100" max="4100" width="13.44140625" style="40" customWidth="1"/>
-    <col min="4101" max="4101" width="74.6640625" style="40" customWidth="1"/>
-    <col min="4102" max="4352" width="14.77734375" style="40"/>
-    <col min="4353" max="4353" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="4354" max="4354" width="33.6640625" style="40" customWidth="1"/>
-    <col min="4355" max="4355" width="14.6640625" style="40" customWidth="1"/>
-    <col min="4356" max="4356" width="13.44140625" style="40" customWidth="1"/>
-    <col min="4357" max="4357" width="74.6640625" style="40" customWidth="1"/>
-    <col min="4358" max="4608" width="14.77734375" style="40"/>
-    <col min="4609" max="4609" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="4610" max="4610" width="33.6640625" style="40" customWidth="1"/>
-    <col min="4611" max="4611" width="14.6640625" style="40" customWidth="1"/>
-    <col min="4612" max="4612" width="13.44140625" style="40" customWidth="1"/>
-    <col min="4613" max="4613" width="74.6640625" style="40" customWidth="1"/>
-    <col min="4614" max="4864" width="14.77734375" style="40"/>
-    <col min="4865" max="4865" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="4866" max="4866" width="33.6640625" style="40" customWidth="1"/>
-    <col min="4867" max="4867" width="14.6640625" style="40" customWidth="1"/>
-    <col min="4868" max="4868" width="13.44140625" style="40" customWidth="1"/>
-    <col min="4869" max="4869" width="74.6640625" style="40" customWidth="1"/>
-    <col min="4870" max="5120" width="14.77734375" style="40"/>
-    <col min="5121" max="5121" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="5122" max="5122" width="33.6640625" style="40" customWidth="1"/>
-    <col min="5123" max="5123" width="14.6640625" style="40" customWidth="1"/>
-    <col min="5124" max="5124" width="13.44140625" style="40" customWidth="1"/>
-    <col min="5125" max="5125" width="74.6640625" style="40" customWidth="1"/>
-    <col min="5126" max="5376" width="14.77734375" style="40"/>
-    <col min="5377" max="5377" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="5378" max="5378" width="33.6640625" style="40" customWidth="1"/>
-    <col min="5379" max="5379" width="14.6640625" style="40" customWidth="1"/>
-    <col min="5380" max="5380" width="13.44140625" style="40" customWidth="1"/>
-    <col min="5381" max="5381" width="74.6640625" style="40" customWidth="1"/>
-    <col min="5382" max="5632" width="14.77734375" style="40"/>
-    <col min="5633" max="5633" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="5634" max="5634" width="33.6640625" style="40" customWidth="1"/>
-    <col min="5635" max="5635" width="14.6640625" style="40" customWidth="1"/>
-    <col min="5636" max="5636" width="13.44140625" style="40" customWidth="1"/>
-    <col min="5637" max="5637" width="74.6640625" style="40" customWidth="1"/>
-    <col min="5638" max="5888" width="14.77734375" style="40"/>
-    <col min="5889" max="5889" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="5890" max="5890" width="33.6640625" style="40" customWidth="1"/>
-    <col min="5891" max="5891" width="14.6640625" style="40" customWidth="1"/>
-    <col min="5892" max="5892" width="13.44140625" style="40" customWidth="1"/>
-    <col min="5893" max="5893" width="74.6640625" style="40" customWidth="1"/>
-    <col min="5894" max="6144" width="14.77734375" style="40"/>
-    <col min="6145" max="6145" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="6146" max="6146" width="33.6640625" style="40" customWidth="1"/>
-    <col min="6147" max="6147" width="14.6640625" style="40" customWidth="1"/>
-    <col min="6148" max="6148" width="13.44140625" style="40" customWidth="1"/>
-    <col min="6149" max="6149" width="74.6640625" style="40" customWidth="1"/>
-    <col min="6150" max="6400" width="14.77734375" style="40"/>
-    <col min="6401" max="6401" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="6402" max="6402" width="33.6640625" style="40" customWidth="1"/>
-    <col min="6403" max="6403" width="14.6640625" style="40" customWidth="1"/>
-    <col min="6404" max="6404" width="13.44140625" style="40" customWidth="1"/>
-    <col min="6405" max="6405" width="74.6640625" style="40" customWidth="1"/>
-    <col min="6406" max="6656" width="14.77734375" style="40"/>
-    <col min="6657" max="6657" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="6658" max="6658" width="33.6640625" style="40" customWidth="1"/>
-    <col min="6659" max="6659" width="14.6640625" style="40" customWidth="1"/>
-    <col min="6660" max="6660" width="13.44140625" style="40" customWidth="1"/>
-    <col min="6661" max="6661" width="74.6640625" style="40" customWidth="1"/>
-    <col min="6662" max="6912" width="14.77734375" style="40"/>
-    <col min="6913" max="6913" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="6914" max="6914" width="33.6640625" style="40" customWidth="1"/>
-    <col min="6915" max="6915" width="14.6640625" style="40" customWidth="1"/>
-    <col min="6916" max="6916" width="13.44140625" style="40" customWidth="1"/>
-    <col min="6917" max="6917" width="74.6640625" style="40" customWidth="1"/>
-    <col min="6918" max="7168" width="14.77734375" style="40"/>
-    <col min="7169" max="7169" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="7170" max="7170" width="33.6640625" style="40" customWidth="1"/>
-    <col min="7171" max="7171" width="14.6640625" style="40" customWidth="1"/>
-    <col min="7172" max="7172" width="13.44140625" style="40" customWidth="1"/>
-    <col min="7173" max="7173" width="74.6640625" style="40" customWidth="1"/>
-    <col min="7174" max="7424" width="14.77734375" style="40"/>
-    <col min="7425" max="7425" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="7426" max="7426" width="33.6640625" style="40" customWidth="1"/>
-    <col min="7427" max="7427" width="14.6640625" style="40" customWidth="1"/>
-    <col min="7428" max="7428" width="13.44140625" style="40" customWidth="1"/>
-    <col min="7429" max="7429" width="74.6640625" style="40" customWidth="1"/>
-    <col min="7430" max="7680" width="14.77734375" style="40"/>
-    <col min="7681" max="7681" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="7682" max="7682" width="33.6640625" style="40" customWidth="1"/>
-    <col min="7683" max="7683" width="14.6640625" style="40" customWidth="1"/>
-    <col min="7684" max="7684" width="13.44140625" style="40" customWidth="1"/>
-    <col min="7685" max="7685" width="74.6640625" style="40" customWidth="1"/>
-    <col min="7686" max="7936" width="14.77734375" style="40"/>
-    <col min="7937" max="7937" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="7938" max="7938" width="33.6640625" style="40" customWidth="1"/>
-    <col min="7939" max="7939" width="14.6640625" style="40" customWidth="1"/>
-    <col min="7940" max="7940" width="13.44140625" style="40" customWidth="1"/>
-    <col min="7941" max="7941" width="74.6640625" style="40" customWidth="1"/>
-    <col min="7942" max="8192" width="14.77734375" style="40"/>
-    <col min="8193" max="8193" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="8194" max="8194" width="33.6640625" style="40" customWidth="1"/>
-    <col min="8195" max="8195" width="14.6640625" style="40" customWidth="1"/>
-    <col min="8196" max="8196" width="13.44140625" style="40" customWidth="1"/>
-    <col min="8197" max="8197" width="74.6640625" style="40" customWidth="1"/>
-    <col min="8198" max="8448" width="14.77734375" style="40"/>
-    <col min="8449" max="8449" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="8450" max="8450" width="33.6640625" style="40" customWidth="1"/>
-    <col min="8451" max="8451" width="14.6640625" style="40" customWidth="1"/>
-    <col min="8452" max="8452" width="13.44140625" style="40" customWidth="1"/>
-    <col min="8453" max="8453" width="74.6640625" style="40" customWidth="1"/>
-    <col min="8454" max="8704" width="14.77734375" style="40"/>
-    <col min="8705" max="8705" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="8706" max="8706" width="33.6640625" style="40" customWidth="1"/>
-    <col min="8707" max="8707" width="14.6640625" style="40" customWidth="1"/>
-    <col min="8708" max="8708" width="13.44140625" style="40" customWidth="1"/>
-    <col min="8709" max="8709" width="74.6640625" style="40" customWidth="1"/>
-    <col min="8710" max="8960" width="14.77734375" style="40"/>
-    <col min="8961" max="8961" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="8962" max="8962" width="33.6640625" style="40" customWidth="1"/>
-    <col min="8963" max="8963" width="14.6640625" style="40" customWidth="1"/>
-    <col min="8964" max="8964" width="13.44140625" style="40" customWidth="1"/>
-    <col min="8965" max="8965" width="74.6640625" style="40" customWidth="1"/>
-    <col min="8966" max="9216" width="14.77734375" style="40"/>
-    <col min="9217" max="9217" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="9218" max="9218" width="33.6640625" style="40" customWidth="1"/>
-    <col min="9219" max="9219" width="14.6640625" style="40" customWidth="1"/>
-    <col min="9220" max="9220" width="13.44140625" style="40" customWidth="1"/>
-    <col min="9221" max="9221" width="74.6640625" style="40" customWidth="1"/>
-    <col min="9222" max="9472" width="14.77734375" style="40"/>
-    <col min="9473" max="9473" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="9474" max="9474" width="33.6640625" style="40" customWidth="1"/>
-    <col min="9475" max="9475" width="14.6640625" style="40" customWidth="1"/>
-    <col min="9476" max="9476" width="13.44140625" style="40" customWidth="1"/>
-    <col min="9477" max="9477" width="74.6640625" style="40" customWidth="1"/>
-    <col min="9478" max="9728" width="14.77734375" style="40"/>
-    <col min="9729" max="9729" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="9730" max="9730" width="33.6640625" style="40" customWidth="1"/>
-    <col min="9731" max="9731" width="14.6640625" style="40" customWidth="1"/>
-    <col min="9732" max="9732" width="13.44140625" style="40" customWidth="1"/>
-    <col min="9733" max="9733" width="74.6640625" style="40" customWidth="1"/>
-    <col min="9734" max="9984" width="14.77734375" style="40"/>
-    <col min="9985" max="9985" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="9986" max="9986" width="33.6640625" style="40" customWidth="1"/>
-    <col min="9987" max="9987" width="14.6640625" style="40" customWidth="1"/>
-    <col min="9988" max="9988" width="13.44140625" style="40" customWidth="1"/>
-    <col min="9989" max="9989" width="74.6640625" style="40" customWidth="1"/>
-    <col min="9990" max="10240" width="14.77734375" style="40"/>
-    <col min="10241" max="10241" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="10242" max="10242" width="33.6640625" style="40" customWidth="1"/>
-    <col min="10243" max="10243" width="14.6640625" style="40" customWidth="1"/>
-    <col min="10244" max="10244" width="13.44140625" style="40" customWidth="1"/>
-    <col min="10245" max="10245" width="74.6640625" style="40" customWidth="1"/>
-    <col min="10246" max="10496" width="14.77734375" style="40"/>
-    <col min="10497" max="10497" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="10498" max="10498" width="33.6640625" style="40" customWidth="1"/>
-    <col min="10499" max="10499" width="14.6640625" style="40" customWidth="1"/>
-    <col min="10500" max="10500" width="13.44140625" style="40" customWidth="1"/>
-    <col min="10501" max="10501" width="74.6640625" style="40" customWidth="1"/>
-    <col min="10502" max="10752" width="14.77734375" style="40"/>
-    <col min="10753" max="10753" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="10754" max="10754" width="33.6640625" style="40" customWidth="1"/>
-    <col min="10755" max="10755" width="14.6640625" style="40" customWidth="1"/>
-    <col min="10756" max="10756" width="13.44140625" style="40" customWidth="1"/>
-    <col min="10757" max="10757" width="74.6640625" style="40" customWidth="1"/>
-    <col min="10758" max="11008" width="14.77734375" style="40"/>
-    <col min="11009" max="11009" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="11010" max="11010" width="33.6640625" style="40" customWidth="1"/>
-    <col min="11011" max="11011" width="14.6640625" style="40" customWidth="1"/>
-    <col min="11012" max="11012" width="13.44140625" style="40" customWidth="1"/>
-    <col min="11013" max="11013" width="74.6640625" style="40" customWidth="1"/>
-    <col min="11014" max="11264" width="14.77734375" style="40"/>
-    <col min="11265" max="11265" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="11266" max="11266" width="33.6640625" style="40" customWidth="1"/>
-    <col min="11267" max="11267" width="14.6640625" style="40" customWidth="1"/>
-    <col min="11268" max="11268" width="13.44140625" style="40" customWidth="1"/>
-    <col min="11269" max="11269" width="74.6640625" style="40" customWidth="1"/>
-    <col min="11270" max="11520" width="14.77734375" style="40"/>
-    <col min="11521" max="11521" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="11522" max="11522" width="33.6640625" style="40" customWidth="1"/>
-    <col min="11523" max="11523" width="14.6640625" style="40" customWidth="1"/>
-    <col min="11524" max="11524" width="13.44140625" style="40" customWidth="1"/>
-    <col min="11525" max="11525" width="74.6640625" style="40" customWidth="1"/>
-    <col min="11526" max="11776" width="14.77734375" style="40"/>
-    <col min="11777" max="11777" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="11778" max="11778" width="33.6640625" style="40" customWidth="1"/>
-    <col min="11779" max="11779" width="14.6640625" style="40" customWidth="1"/>
-    <col min="11780" max="11780" width="13.44140625" style="40" customWidth="1"/>
-    <col min="11781" max="11781" width="74.6640625" style="40" customWidth="1"/>
-    <col min="11782" max="12032" width="14.77734375" style="40"/>
-    <col min="12033" max="12033" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="12034" max="12034" width="33.6640625" style="40" customWidth="1"/>
-    <col min="12035" max="12035" width="14.6640625" style="40" customWidth="1"/>
-    <col min="12036" max="12036" width="13.44140625" style="40" customWidth="1"/>
-    <col min="12037" max="12037" width="74.6640625" style="40" customWidth="1"/>
-    <col min="12038" max="12288" width="14.77734375" style="40"/>
-    <col min="12289" max="12289" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="12290" max="12290" width="33.6640625" style="40" customWidth="1"/>
-    <col min="12291" max="12291" width="14.6640625" style="40" customWidth="1"/>
-    <col min="12292" max="12292" width="13.44140625" style="40" customWidth="1"/>
-    <col min="12293" max="12293" width="74.6640625" style="40" customWidth="1"/>
-    <col min="12294" max="12544" width="14.77734375" style="40"/>
-    <col min="12545" max="12545" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="12546" max="12546" width="33.6640625" style="40" customWidth="1"/>
-    <col min="12547" max="12547" width="14.6640625" style="40" customWidth="1"/>
-    <col min="12548" max="12548" width="13.44140625" style="40" customWidth="1"/>
-    <col min="12549" max="12549" width="74.6640625" style="40" customWidth="1"/>
-    <col min="12550" max="12800" width="14.77734375" style="40"/>
-    <col min="12801" max="12801" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="12802" max="12802" width="33.6640625" style="40" customWidth="1"/>
-    <col min="12803" max="12803" width="14.6640625" style="40" customWidth="1"/>
-    <col min="12804" max="12804" width="13.44140625" style="40" customWidth="1"/>
-    <col min="12805" max="12805" width="74.6640625" style="40" customWidth="1"/>
-    <col min="12806" max="13056" width="14.77734375" style="40"/>
-    <col min="13057" max="13057" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="13058" max="13058" width="33.6640625" style="40" customWidth="1"/>
-    <col min="13059" max="13059" width="14.6640625" style="40" customWidth="1"/>
-    <col min="13060" max="13060" width="13.44140625" style="40" customWidth="1"/>
-    <col min="13061" max="13061" width="74.6640625" style="40" customWidth="1"/>
-    <col min="13062" max="13312" width="14.77734375" style="40"/>
-    <col min="13313" max="13313" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="13314" max="13314" width="33.6640625" style="40" customWidth="1"/>
-    <col min="13315" max="13315" width="14.6640625" style="40" customWidth="1"/>
-    <col min="13316" max="13316" width="13.44140625" style="40" customWidth="1"/>
-    <col min="13317" max="13317" width="74.6640625" style="40" customWidth="1"/>
-    <col min="13318" max="13568" width="14.77734375" style="40"/>
-    <col min="13569" max="13569" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="13570" max="13570" width="33.6640625" style="40" customWidth="1"/>
-    <col min="13571" max="13571" width="14.6640625" style="40" customWidth="1"/>
-    <col min="13572" max="13572" width="13.44140625" style="40" customWidth="1"/>
-    <col min="13573" max="13573" width="74.6640625" style="40" customWidth="1"/>
-    <col min="13574" max="13824" width="14.77734375" style="40"/>
-    <col min="13825" max="13825" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="13826" max="13826" width="33.6640625" style="40" customWidth="1"/>
-    <col min="13827" max="13827" width="14.6640625" style="40" customWidth="1"/>
-    <col min="13828" max="13828" width="13.44140625" style="40" customWidth="1"/>
-    <col min="13829" max="13829" width="74.6640625" style="40" customWidth="1"/>
-    <col min="13830" max="14080" width="14.77734375" style="40"/>
-    <col min="14081" max="14081" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="14082" max="14082" width="33.6640625" style="40" customWidth="1"/>
-    <col min="14083" max="14083" width="14.6640625" style="40" customWidth="1"/>
-    <col min="14084" max="14084" width="13.44140625" style="40" customWidth="1"/>
-    <col min="14085" max="14085" width="74.6640625" style="40" customWidth="1"/>
-    <col min="14086" max="14336" width="14.77734375" style="40"/>
-    <col min="14337" max="14337" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="14338" max="14338" width="33.6640625" style="40" customWidth="1"/>
-    <col min="14339" max="14339" width="14.6640625" style="40" customWidth="1"/>
-    <col min="14340" max="14340" width="13.44140625" style="40" customWidth="1"/>
-    <col min="14341" max="14341" width="74.6640625" style="40" customWidth="1"/>
-    <col min="14342" max="14592" width="14.77734375" style="40"/>
-    <col min="14593" max="14593" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="14594" max="14594" width="33.6640625" style="40" customWidth="1"/>
-    <col min="14595" max="14595" width="14.6640625" style="40" customWidth="1"/>
-    <col min="14596" max="14596" width="13.44140625" style="40" customWidth="1"/>
-    <col min="14597" max="14597" width="74.6640625" style="40" customWidth="1"/>
-    <col min="14598" max="14848" width="14.77734375" style="40"/>
-    <col min="14849" max="14849" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="14850" max="14850" width="33.6640625" style="40" customWidth="1"/>
-    <col min="14851" max="14851" width="14.6640625" style="40" customWidth="1"/>
-    <col min="14852" max="14852" width="13.44140625" style="40" customWidth="1"/>
-    <col min="14853" max="14853" width="74.6640625" style="40" customWidth="1"/>
-    <col min="14854" max="15104" width="14.77734375" style="40"/>
-    <col min="15105" max="15105" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="15106" max="15106" width="33.6640625" style="40" customWidth="1"/>
-    <col min="15107" max="15107" width="14.6640625" style="40" customWidth="1"/>
-    <col min="15108" max="15108" width="13.44140625" style="40" customWidth="1"/>
-    <col min="15109" max="15109" width="74.6640625" style="40" customWidth="1"/>
-    <col min="15110" max="15360" width="14.77734375" style="40"/>
-    <col min="15361" max="15361" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="15362" max="15362" width="33.6640625" style="40" customWidth="1"/>
-    <col min="15363" max="15363" width="14.6640625" style="40" customWidth="1"/>
-    <col min="15364" max="15364" width="13.44140625" style="40" customWidth="1"/>
-    <col min="15365" max="15365" width="74.6640625" style="40" customWidth="1"/>
-    <col min="15366" max="15616" width="14.77734375" style="40"/>
-    <col min="15617" max="15617" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="15618" max="15618" width="33.6640625" style="40" customWidth="1"/>
-    <col min="15619" max="15619" width="14.6640625" style="40" customWidth="1"/>
-    <col min="15620" max="15620" width="13.44140625" style="40" customWidth="1"/>
-    <col min="15621" max="15621" width="74.6640625" style="40" customWidth="1"/>
-    <col min="15622" max="15872" width="14.77734375" style="40"/>
-    <col min="15873" max="15873" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="15874" max="15874" width="33.6640625" style="40" customWidth="1"/>
-    <col min="15875" max="15875" width="14.6640625" style="40" customWidth="1"/>
-    <col min="15876" max="15876" width="13.44140625" style="40" customWidth="1"/>
-    <col min="15877" max="15877" width="74.6640625" style="40" customWidth="1"/>
-    <col min="15878" max="16128" width="14.77734375" style="40"/>
-    <col min="16129" max="16129" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="16130" max="16130" width="33.6640625" style="40" customWidth="1"/>
-    <col min="16131" max="16131" width="14.6640625" style="40" customWidth="1"/>
-    <col min="16132" max="16132" width="13.44140625" style="40" customWidth="1"/>
-    <col min="16133" max="16133" width="74.6640625" style="40" customWidth="1"/>
-    <col min="16134" max="16384" width="14.77734375" style="40"/>
+    <col min="1" max="1" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.6328125" style="40" customWidth="1"/>
+    <col min="3" max="3" width="26.81640625" style="40" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" style="40" customWidth="1"/>
+    <col min="5" max="5" width="87.453125" style="40" customWidth="1"/>
+    <col min="6" max="256" width="14.81640625" style="40"/>
+    <col min="257" max="257" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="258" max="258" width="33.6328125" style="40" customWidth="1"/>
+    <col min="259" max="259" width="14.6328125" style="40" customWidth="1"/>
+    <col min="260" max="260" width="13.453125" style="40" customWidth="1"/>
+    <col min="261" max="261" width="74.6328125" style="40" customWidth="1"/>
+    <col min="262" max="512" width="14.81640625" style="40"/>
+    <col min="513" max="513" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="514" max="514" width="33.6328125" style="40" customWidth="1"/>
+    <col min="515" max="515" width="14.6328125" style="40" customWidth="1"/>
+    <col min="516" max="516" width="13.453125" style="40" customWidth="1"/>
+    <col min="517" max="517" width="74.6328125" style="40" customWidth="1"/>
+    <col min="518" max="768" width="14.81640625" style="40"/>
+    <col min="769" max="769" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="770" max="770" width="33.6328125" style="40" customWidth="1"/>
+    <col min="771" max="771" width="14.6328125" style="40" customWidth="1"/>
+    <col min="772" max="772" width="13.453125" style="40" customWidth="1"/>
+    <col min="773" max="773" width="74.6328125" style="40" customWidth="1"/>
+    <col min="774" max="1024" width="14.81640625" style="40"/>
+    <col min="1025" max="1025" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="1026" max="1026" width="33.6328125" style="40" customWidth="1"/>
+    <col min="1027" max="1027" width="14.6328125" style="40" customWidth="1"/>
+    <col min="1028" max="1028" width="13.453125" style="40" customWidth="1"/>
+    <col min="1029" max="1029" width="74.6328125" style="40" customWidth="1"/>
+    <col min="1030" max="1280" width="14.81640625" style="40"/>
+    <col min="1281" max="1281" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="1282" max="1282" width="33.6328125" style="40" customWidth="1"/>
+    <col min="1283" max="1283" width="14.6328125" style="40" customWidth="1"/>
+    <col min="1284" max="1284" width="13.453125" style="40" customWidth="1"/>
+    <col min="1285" max="1285" width="74.6328125" style="40" customWidth="1"/>
+    <col min="1286" max="1536" width="14.81640625" style="40"/>
+    <col min="1537" max="1537" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="1538" max="1538" width="33.6328125" style="40" customWidth="1"/>
+    <col min="1539" max="1539" width="14.6328125" style="40" customWidth="1"/>
+    <col min="1540" max="1540" width="13.453125" style="40" customWidth="1"/>
+    <col min="1541" max="1541" width="74.6328125" style="40" customWidth="1"/>
+    <col min="1542" max="1792" width="14.81640625" style="40"/>
+    <col min="1793" max="1793" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="1794" max="1794" width="33.6328125" style="40" customWidth="1"/>
+    <col min="1795" max="1795" width="14.6328125" style="40" customWidth="1"/>
+    <col min="1796" max="1796" width="13.453125" style="40" customWidth="1"/>
+    <col min="1797" max="1797" width="74.6328125" style="40" customWidth="1"/>
+    <col min="1798" max="2048" width="14.81640625" style="40"/>
+    <col min="2049" max="2049" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="2050" max="2050" width="33.6328125" style="40" customWidth="1"/>
+    <col min="2051" max="2051" width="14.6328125" style="40" customWidth="1"/>
+    <col min="2052" max="2052" width="13.453125" style="40" customWidth="1"/>
+    <col min="2053" max="2053" width="74.6328125" style="40" customWidth="1"/>
+    <col min="2054" max="2304" width="14.81640625" style="40"/>
+    <col min="2305" max="2305" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="2306" max="2306" width="33.6328125" style="40" customWidth="1"/>
+    <col min="2307" max="2307" width="14.6328125" style="40" customWidth="1"/>
+    <col min="2308" max="2308" width="13.453125" style="40" customWidth="1"/>
+    <col min="2309" max="2309" width="74.6328125" style="40" customWidth="1"/>
+    <col min="2310" max="2560" width="14.81640625" style="40"/>
+    <col min="2561" max="2561" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="2562" max="2562" width="33.6328125" style="40" customWidth="1"/>
+    <col min="2563" max="2563" width="14.6328125" style="40" customWidth="1"/>
+    <col min="2564" max="2564" width="13.453125" style="40" customWidth="1"/>
+    <col min="2565" max="2565" width="74.6328125" style="40" customWidth="1"/>
+    <col min="2566" max="2816" width="14.81640625" style="40"/>
+    <col min="2817" max="2817" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="2818" max="2818" width="33.6328125" style="40" customWidth="1"/>
+    <col min="2819" max="2819" width="14.6328125" style="40" customWidth="1"/>
+    <col min="2820" max="2820" width="13.453125" style="40" customWidth="1"/>
+    <col min="2821" max="2821" width="74.6328125" style="40" customWidth="1"/>
+    <col min="2822" max="3072" width="14.81640625" style="40"/>
+    <col min="3073" max="3073" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="3074" max="3074" width="33.6328125" style="40" customWidth="1"/>
+    <col min="3075" max="3075" width="14.6328125" style="40" customWidth="1"/>
+    <col min="3076" max="3076" width="13.453125" style="40" customWidth="1"/>
+    <col min="3077" max="3077" width="74.6328125" style="40" customWidth="1"/>
+    <col min="3078" max="3328" width="14.81640625" style="40"/>
+    <col min="3329" max="3329" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="3330" max="3330" width="33.6328125" style="40" customWidth="1"/>
+    <col min="3331" max="3331" width="14.6328125" style="40" customWidth="1"/>
+    <col min="3332" max="3332" width="13.453125" style="40" customWidth="1"/>
+    <col min="3333" max="3333" width="74.6328125" style="40" customWidth="1"/>
+    <col min="3334" max="3584" width="14.81640625" style="40"/>
+    <col min="3585" max="3585" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="3586" max="3586" width="33.6328125" style="40" customWidth="1"/>
+    <col min="3587" max="3587" width="14.6328125" style="40" customWidth="1"/>
+    <col min="3588" max="3588" width="13.453125" style="40" customWidth="1"/>
+    <col min="3589" max="3589" width="74.6328125" style="40" customWidth="1"/>
+    <col min="3590" max="3840" width="14.81640625" style="40"/>
+    <col min="3841" max="3841" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="3842" max="3842" width="33.6328125" style="40" customWidth="1"/>
+    <col min="3843" max="3843" width="14.6328125" style="40" customWidth="1"/>
+    <col min="3844" max="3844" width="13.453125" style="40" customWidth="1"/>
+    <col min="3845" max="3845" width="74.6328125" style="40" customWidth="1"/>
+    <col min="3846" max="4096" width="14.81640625" style="40"/>
+    <col min="4097" max="4097" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="4098" max="4098" width="33.6328125" style="40" customWidth="1"/>
+    <col min="4099" max="4099" width="14.6328125" style="40" customWidth="1"/>
+    <col min="4100" max="4100" width="13.453125" style="40" customWidth="1"/>
+    <col min="4101" max="4101" width="74.6328125" style="40" customWidth="1"/>
+    <col min="4102" max="4352" width="14.81640625" style="40"/>
+    <col min="4353" max="4353" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="4354" max="4354" width="33.6328125" style="40" customWidth="1"/>
+    <col min="4355" max="4355" width="14.6328125" style="40" customWidth="1"/>
+    <col min="4356" max="4356" width="13.453125" style="40" customWidth="1"/>
+    <col min="4357" max="4357" width="74.6328125" style="40" customWidth="1"/>
+    <col min="4358" max="4608" width="14.81640625" style="40"/>
+    <col min="4609" max="4609" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="4610" max="4610" width="33.6328125" style="40" customWidth="1"/>
+    <col min="4611" max="4611" width="14.6328125" style="40" customWidth="1"/>
+    <col min="4612" max="4612" width="13.453125" style="40" customWidth="1"/>
+    <col min="4613" max="4613" width="74.6328125" style="40" customWidth="1"/>
+    <col min="4614" max="4864" width="14.81640625" style="40"/>
+    <col min="4865" max="4865" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="4866" max="4866" width="33.6328125" style="40" customWidth="1"/>
+    <col min="4867" max="4867" width="14.6328125" style="40" customWidth="1"/>
+    <col min="4868" max="4868" width="13.453125" style="40" customWidth="1"/>
+    <col min="4869" max="4869" width="74.6328125" style="40" customWidth="1"/>
+    <col min="4870" max="5120" width="14.81640625" style="40"/>
+    <col min="5121" max="5121" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="5122" max="5122" width="33.6328125" style="40" customWidth="1"/>
+    <col min="5123" max="5123" width="14.6328125" style="40" customWidth="1"/>
+    <col min="5124" max="5124" width="13.453125" style="40" customWidth="1"/>
+    <col min="5125" max="5125" width="74.6328125" style="40" customWidth="1"/>
+    <col min="5126" max="5376" width="14.81640625" style="40"/>
+    <col min="5377" max="5377" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="5378" max="5378" width="33.6328125" style="40" customWidth="1"/>
+    <col min="5379" max="5379" width="14.6328125" style="40" customWidth="1"/>
+    <col min="5380" max="5380" width="13.453125" style="40" customWidth="1"/>
+    <col min="5381" max="5381" width="74.6328125" style="40" customWidth="1"/>
+    <col min="5382" max="5632" width="14.81640625" style="40"/>
+    <col min="5633" max="5633" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="5634" max="5634" width="33.6328125" style="40" customWidth="1"/>
+    <col min="5635" max="5635" width="14.6328125" style="40" customWidth="1"/>
+    <col min="5636" max="5636" width="13.453125" style="40" customWidth="1"/>
+    <col min="5637" max="5637" width="74.6328125" style="40" customWidth="1"/>
+    <col min="5638" max="5888" width="14.81640625" style="40"/>
+    <col min="5889" max="5889" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="5890" max="5890" width="33.6328125" style="40" customWidth="1"/>
+    <col min="5891" max="5891" width="14.6328125" style="40" customWidth="1"/>
+    <col min="5892" max="5892" width="13.453125" style="40" customWidth="1"/>
+    <col min="5893" max="5893" width="74.6328125" style="40" customWidth="1"/>
+    <col min="5894" max="6144" width="14.81640625" style="40"/>
+    <col min="6145" max="6145" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="6146" max="6146" width="33.6328125" style="40" customWidth="1"/>
+    <col min="6147" max="6147" width="14.6328125" style="40" customWidth="1"/>
+    <col min="6148" max="6148" width="13.453125" style="40" customWidth="1"/>
+    <col min="6149" max="6149" width="74.6328125" style="40" customWidth="1"/>
+    <col min="6150" max="6400" width="14.81640625" style="40"/>
+    <col min="6401" max="6401" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="6402" max="6402" width="33.6328125" style="40" customWidth="1"/>
+    <col min="6403" max="6403" width="14.6328125" style="40" customWidth="1"/>
+    <col min="6404" max="6404" width="13.453125" style="40" customWidth="1"/>
+    <col min="6405" max="6405" width="74.6328125" style="40" customWidth="1"/>
+    <col min="6406" max="6656" width="14.81640625" style="40"/>
+    <col min="6657" max="6657" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="6658" max="6658" width="33.6328125" style="40" customWidth="1"/>
+    <col min="6659" max="6659" width="14.6328125" style="40" customWidth="1"/>
+    <col min="6660" max="6660" width="13.453125" style="40" customWidth="1"/>
+    <col min="6661" max="6661" width="74.6328125" style="40" customWidth="1"/>
+    <col min="6662" max="6912" width="14.81640625" style="40"/>
+    <col min="6913" max="6913" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="6914" max="6914" width="33.6328125" style="40" customWidth="1"/>
+    <col min="6915" max="6915" width="14.6328125" style="40" customWidth="1"/>
+    <col min="6916" max="6916" width="13.453125" style="40" customWidth="1"/>
+    <col min="6917" max="6917" width="74.6328125" style="40" customWidth="1"/>
+    <col min="6918" max="7168" width="14.81640625" style="40"/>
+    <col min="7169" max="7169" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="7170" max="7170" width="33.6328125" style="40" customWidth="1"/>
+    <col min="7171" max="7171" width="14.6328125" style="40" customWidth="1"/>
+    <col min="7172" max="7172" width="13.453125" style="40" customWidth="1"/>
+    <col min="7173" max="7173" width="74.6328125" style="40" customWidth="1"/>
+    <col min="7174" max="7424" width="14.81640625" style="40"/>
+    <col min="7425" max="7425" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="7426" max="7426" width="33.6328125" style="40" customWidth="1"/>
+    <col min="7427" max="7427" width="14.6328125" style="40" customWidth="1"/>
+    <col min="7428" max="7428" width="13.453125" style="40" customWidth="1"/>
+    <col min="7429" max="7429" width="74.6328125" style="40" customWidth="1"/>
+    <col min="7430" max="7680" width="14.81640625" style="40"/>
+    <col min="7681" max="7681" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="7682" max="7682" width="33.6328125" style="40" customWidth="1"/>
+    <col min="7683" max="7683" width="14.6328125" style="40" customWidth="1"/>
+    <col min="7684" max="7684" width="13.453125" style="40" customWidth="1"/>
+    <col min="7685" max="7685" width="74.6328125" style="40" customWidth="1"/>
+    <col min="7686" max="7936" width="14.81640625" style="40"/>
+    <col min="7937" max="7937" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="7938" max="7938" width="33.6328125" style="40" customWidth="1"/>
+    <col min="7939" max="7939" width="14.6328125" style="40" customWidth="1"/>
+    <col min="7940" max="7940" width="13.453125" style="40" customWidth="1"/>
+    <col min="7941" max="7941" width="74.6328125" style="40" customWidth="1"/>
+    <col min="7942" max="8192" width="14.81640625" style="40"/>
+    <col min="8193" max="8193" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="8194" max="8194" width="33.6328125" style="40" customWidth="1"/>
+    <col min="8195" max="8195" width="14.6328125" style="40" customWidth="1"/>
+    <col min="8196" max="8196" width="13.453125" style="40" customWidth="1"/>
+    <col min="8197" max="8197" width="74.6328125" style="40" customWidth="1"/>
+    <col min="8198" max="8448" width="14.81640625" style="40"/>
+    <col min="8449" max="8449" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="8450" max="8450" width="33.6328125" style="40" customWidth="1"/>
+    <col min="8451" max="8451" width="14.6328125" style="40" customWidth="1"/>
+    <col min="8452" max="8452" width="13.453125" style="40" customWidth="1"/>
+    <col min="8453" max="8453" width="74.6328125" style="40" customWidth="1"/>
+    <col min="8454" max="8704" width="14.81640625" style="40"/>
+    <col min="8705" max="8705" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="8706" max="8706" width="33.6328125" style="40" customWidth="1"/>
+    <col min="8707" max="8707" width="14.6328125" style="40" customWidth="1"/>
+    <col min="8708" max="8708" width="13.453125" style="40" customWidth="1"/>
+    <col min="8709" max="8709" width="74.6328125" style="40" customWidth="1"/>
+    <col min="8710" max="8960" width="14.81640625" style="40"/>
+    <col min="8961" max="8961" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="8962" max="8962" width="33.6328125" style="40" customWidth="1"/>
+    <col min="8963" max="8963" width="14.6328125" style="40" customWidth="1"/>
+    <col min="8964" max="8964" width="13.453125" style="40" customWidth="1"/>
+    <col min="8965" max="8965" width="74.6328125" style="40" customWidth="1"/>
+    <col min="8966" max="9216" width="14.81640625" style="40"/>
+    <col min="9217" max="9217" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="9218" max="9218" width="33.6328125" style="40" customWidth="1"/>
+    <col min="9219" max="9219" width="14.6328125" style="40" customWidth="1"/>
+    <col min="9220" max="9220" width="13.453125" style="40" customWidth="1"/>
+    <col min="9221" max="9221" width="74.6328125" style="40" customWidth="1"/>
+    <col min="9222" max="9472" width="14.81640625" style="40"/>
+    <col min="9473" max="9473" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="9474" max="9474" width="33.6328125" style="40" customWidth="1"/>
+    <col min="9475" max="9475" width="14.6328125" style="40" customWidth="1"/>
+    <col min="9476" max="9476" width="13.453125" style="40" customWidth="1"/>
+    <col min="9477" max="9477" width="74.6328125" style="40" customWidth="1"/>
+    <col min="9478" max="9728" width="14.81640625" style="40"/>
+    <col min="9729" max="9729" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="9730" max="9730" width="33.6328125" style="40" customWidth="1"/>
+    <col min="9731" max="9731" width="14.6328125" style="40" customWidth="1"/>
+    <col min="9732" max="9732" width="13.453125" style="40" customWidth="1"/>
+    <col min="9733" max="9733" width="74.6328125" style="40" customWidth="1"/>
+    <col min="9734" max="9984" width="14.81640625" style="40"/>
+    <col min="9985" max="9985" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="9986" max="9986" width="33.6328125" style="40" customWidth="1"/>
+    <col min="9987" max="9987" width="14.6328125" style="40" customWidth="1"/>
+    <col min="9988" max="9988" width="13.453125" style="40" customWidth="1"/>
+    <col min="9989" max="9989" width="74.6328125" style="40" customWidth="1"/>
+    <col min="9990" max="10240" width="14.81640625" style="40"/>
+    <col min="10241" max="10241" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="10242" max="10242" width="33.6328125" style="40" customWidth="1"/>
+    <col min="10243" max="10243" width="14.6328125" style="40" customWidth="1"/>
+    <col min="10244" max="10244" width="13.453125" style="40" customWidth="1"/>
+    <col min="10245" max="10245" width="74.6328125" style="40" customWidth="1"/>
+    <col min="10246" max="10496" width="14.81640625" style="40"/>
+    <col min="10497" max="10497" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="10498" max="10498" width="33.6328125" style="40" customWidth="1"/>
+    <col min="10499" max="10499" width="14.6328125" style="40" customWidth="1"/>
+    <col min="10500" max="10500" width="13.453125" style="40" customWidth="1"/>
+    <col min="10501" max="10501" width="74.6328125" style="40" customWidth="1"/>
+    <col min="10502" max="10752" width="14.81640625" style="40"/>
+    <col min="10753" max="10753" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="10754" max="10754" width="33.6328125" style="40" customWidth="1"/>
+    <col min="10755" max="10755" width="14.6328125" style="40" customWidth="1"/>
+    <col min="10756" max="10756" width="13.453125" style="40" customWidth="1"/>
+    <col min="10757" max="10757" width="74.6328125" style="40" customWidth="1"/>
+    <col min="10758" max="11008" width="14.81640625" style="40"/>
+    <col min="11009" max="11009" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="11010" max="11010" width="33.6328125" style="40" customWidth="1"/>
+    <col min="11011" max="11011" width="14.6328125" style="40" customWidth="1"/>
+    <col min="11012" max="11012" width="13.453125" style="40" customWidth="1"/>
+    <col min="11013" max="11013" width="74.6328125" style="40" customWidth="1"/>
+    <col min="11014" max="11264" width="14.81640625" style="40"/>
+    <col min="11265" max="11265" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="11266" max="11266" width="33.6328125" style="40" customWidth="1"/>
+    <col min="11267" max="11267" width="14.6328125" style="40" customWidth="1"/>
+    <col min="11268" max="11268" width="13.453125" style="40" customWidth="1"/>
+    <col min="11269" max="11269" width="74.6328125" style="40" customWidth="1"/>
+    <col min="11270" max="11520" width="14.81640625" style="40"/>
+    <col min="11521" max="11521" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="11522" max="11522" width="33.6328125" style="40" customWidth="1"/>
+    <col min="11523" max="11523" width="14.6328125" style="40" customWidth="1"/>
+    <col min="11524" max="11524" width="13.453125" style="40" customWidth="1"/>
+    <col min="11525" max="11525" width="74.6328125" style="40" customWidth="1"/>
+    <col min="11526" max="11776" width="14.81640625" style="40"/>
+    <col min="11777" max="11777" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="11778" max="11778" width="33.6328125" style="40" customWidth="1"/>
+    <col min="11779" max="11779" width="14.6328125" style="40" customWidth="1"/>
+    <col min="11780" max="11780" width="13.453125" style="40" customWidth="1"/>
+    <col min="11781" max="11781" width="74.6328125" style="40" customWidth="1"/>
+    <col min="11782" max="12032" width="14.81640625" style="40"/>
+    <col min="12033" max="12033" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="12034" max="12034" width="33.6328125" style="40" customWidth="1"/>
+    <col min="12035" max="12035" width="14.6328125" style="40" customWidth="1"/>
+    <col min="12036" max="12036" width="13.453125" style="40" customWidth="1"/>
+    <col min="12037" max="12037" width="74.6328125" style="40" customWidth="1"/>
+    <col min="12038" max="12288" width="14.81640625" style="40"/>
+    <col min="12289" max="12289" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="12290" max="12290" width="33.6328125" style="40" customWidth="1"/>
+    <col min="12291" max="12291" width="14.6328125" style="40" customWidth="1"/>
+    <col min="12292" max="12292" width="13.453125" style="40" customWidth="1"/>
+    <col min="12293" max="12293" width="74.6328125" style="40" customWidth="1"/>
+    <col min="12294" max="12544" width="14.81640625" style="40"/>
+    <col min="12545" max="12545" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="12546" max="12546" width="33.6328125" style="40" customWidth="1"/>
+    <col min="12547" max="12547" width="14.6328125" style="40" customWidth="1"/>
+    <col min="12548" max="12548" width="13.453125" style="40" customWidth="1"/>
+    <col min="12549" max="12549" width="74.6328125" style="40" customWidth="1"/>
+    <col min="12550" max="12800" width="14.81640625" style="40"/>
+    <col min="12801" max="12801" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="12802" max="12802" width="33.6328125" style="40" customWidth="1"/>
+    <col min="12803" max="12803" width="14.6328125" style="40" customWidth="1"/>
+    <col min="12804" max="12804" width="13.453125" style="40" customWidth="1"/>
+    <col min="12805" max="12805" width="74.6328125" style="40" customWidth="1"/>
+    <col min="12806" max="13056" width="14.81640625" style="40"/>
+    <col min="13057" max="13057" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="13058" max="13058" width="33.6328125" style="40" customWidth="1"/>
+    <col min="13059" max="13059" width="14.6328125" style="40" customWidth="1"/>
+    <col min="13060" max="13060" width="13.453125" style="40" customWidth="1"/>
+    <col min="13061" max="13061" width="74.6328125" style="40" customWidth="1"/>
+    <col min="13062" max="13312" width="14.81640625" style="40"/>
+    <col min="13313" max="13313" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="13314" max="13314" width="33.6328125" style="40" customWidth="1"/>
+    <col min="13315" max="13315" width="14.6328125" style="40" customWidth="1"/>
+    <col min="13316" max="13316" width="13.453125" style="40" customWidth="1"/>
+    <col min="13317" max="13317" width="74.6328125" style="40" customWidth="1"/>
+    <col min="13318" max="13568" width="14.81640625" style="40"/>
+    <col min="13569" max="13569" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="13570" max="13570" width="33.6328125" style="40" customWidth="1"/>
+    <col min="13571" max="13571" width="14.6328125" style="40" customWidth="1"/>
+    <col min="13572" max="13572" width="13.453125" style="40" customWidth="1"/>
+    <col min="13573" max="13573" width="74.6328125" style="40" customWidth="1"/>
+    <col min="13574" max="13824" width="14.81640625" style="40"/>
+    <col min="13825" max="13825" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="13826" max="13826" width="33.6328125" style="40" customWidth="1"/>
+    <col min="13827" max="13827" width="14.6328125" style="40" customWidth="1"/>
+    <col min="13828" max="13828" width="13.453125" style="40" customWidth="1"/>
+    <col min="13829" max="13829" width="74.6328125" style="40" customWidth="1"/>
+    <col min="13830" max="14080" width="14.81640625" style="40"/>
+    <col min="14081" max="14081" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="14082" max="14082" width="33.6328125" style="40" customWidth="1"/>
+    <col min="14083" max="14083" width="14.6328125" style="40" customWidth="1"/>
+    <col min="14084" max="14084" width="13.453125" style="40" customWidth="1"/>
+    <col min="14085" max="14085" width="74.6328125" style="40" customWidth="1"/>
+    <col min="14086" max="14336" width="14.81640625" style="40"/>
+    <col min="14337" max="14337" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="14338" max="14338" width="33.6328125" style="40" customWidth="1"/>
+    <col min="14339" max="14339" width="14.6328125" style="40" customWidth="1"/>
+    <col min="14340" max="14340" width="13.453125" style="40" customWidth="1"/>
+    <col min="14341" max="14341" width="74.6328125" style="40" customWidth="1"/>
+    <col min="14342" max="14592" width="14.81640625" style="40"/>
+    <col min="14593" max="14593" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="14594" max="14594" width="33.6328125" style="40" customWidth="1"/>
+    <col min="14595" max="14595" width="14.6328125" style="40" customWidth="1"/>
+    <col min="14596" max="14596" width="13.453125" style="40" customWidth="1"/>
+    <col min="14597" max="14597" width="74.6328125" style="40" customWidth="1"/>
+    <col min="14598" max="14848" width="14.81640625" style="40"/>
+    <col min="14849" max="14849" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="14850" max="14850" width="33.6328125" style="40" customWidth="1"/>
+    <col min="14851" max="14851" width="14.6328125" style="40" customWidth="1"/>
+    <col min="14852" max="14852" width="13.453125" style="40" customWidth="1"/>
+    <col min="14853" max="14853" width="74.6328125" style="40" customWidth="1"/>
+    <col min="14854" max="15104" width="14.81640625" style="40"/>
+    <col min="15105" max="15105" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="15106" max="15106" width="33.6328125" style="40" customWidth="1"/>
+    <col min="15107" max="15107" width="14.6328125" style="40" customWidth="1"/>
+    <col min="15108" max="15108" width="13.453125" style="40" customWidth="1"/>
+    <col min="15109" max="15109" width="74.6328125" style="40" customWidth="1"/>
+    <col min="15110" max="15360" width="14.81640625" style="40"/>
+    <col min="15361" max="15361" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="15362" max="15362" width="33.6328125" style="40" customWidth="1"/>
+    <col min="15363" max="15363" width="14.6328125" style="40" customWidth="1"/>
+    <col min="15364" max="15364" width="13.453125" style="40" customWidth="1"/>
+    <col min="15365" max="15365" width="74.6328125" style="40" customWidth="1"/>
+    <col min="15366" max="15616" width="14.81640625" style="40"/>
+    <col min="15617" max="15617" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="15618" max="15618" width="33.6328125" style="40" customWidth="1"/>
+    <col min="15619" max="15619" width="14.6328125" style="40" customWidth="1"/>
+    <col min="15620" max="15620" width="13.453125" style="40" customWidth="1"/>
+    <col min="15621" max="15621" width="74.6328125" style="40" customWidth="1"/>
+    <col min="15622" max="15872" width="14.81640625" style="40"/>
+    <col min="15873" max="15873" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="15874" max="15874" width="33.6328125" style="40" customWidth="1"/>
+    <col min="15875" max="15875" width="14.6328125" style="40" customWidth="1"/>
+    <col min="15876" max="15876" width="13.453125" style="40" customWidth="1"/>
+    <col min="15877" max="15877" width="74.6328125" style="40" customWidth="1"/>
+    <col min="15878" max="16128" width="14.81640625" style="40"/>
+    <col min="16129" max="16129" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="16130" max="16130" width="33.6328125" style="40" customWidth="1"/>
+    <col min="16131" max="16131" width="14.6328125" style="40" customWidth="1"/>
+    <col min="16132" max="16132" width="13.453125" style="40" customWidth="1"/>
+    <col min="16133" max="16133" width="74.6328125" style="40" customWidth="1"/>
+    <col min="16134" max="16384" width="14.81640625" style="40"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" thickBot="1">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="40.25" customHeight="1" thickBot="1">
       <c r="A1" s="108"/>
       <c r="B1" s="109"/>
       <c r="C1" s="109"/>
       <c r="D1" s="109"/>
       <c r="E1" s="109"/>
     </row>
-    <row r="2" spans="1:5" ht="13.95" customHeight="1">
+    <row r="2" spans="1:5" ht="14" customHeight="1">
       <c r="A2" s="118" t="s">
         <v>64</v>
       </c>
@@ -48246,7 +48211,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14.4" thickBot="1">
+    <row r="3" spans="1:5" ht="14.5" thickBot="1">
       <c r="A3" s="111"/>
       <c r="B3" s="113"/>
       <c r="C3" s="115"/>
@@ -48324,7 +48289,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="14.4" thickBot="1">
+    <row r="9" spans="1:5" ht="14.5" thickBot="1">
       <c r="A9" s="45" t="s">
         <v>153</v>
       </c>
@@ -48339,7 +48304,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="14.4" thickBot="1">
+    <row r="10" spans="1:5" ht="14.5" thickBot="1">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="6"/>
@@ -48417,7 +48382,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="14.4" thickBot="1">
+    <row r="16" spans="1:5" ht="14.5" thickBot="1">
       <c r="A16" s="54" t="s">
         <v>153</v>
       </c>
@@ -48492,7 +48457,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="14.4" thickBot="1">
+    <row r="21" spans="1:5" ht="14.5" thickBot="1">
       <c r="A21" s="45" t="s">
         <v>153</v>
       </c>
@@ -48507,7 +48472,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="14.4" thickBot="1">
+    <row r="22" spans="1:5" ht="14.5" thickBot="1">
       <c r="A22" s="58"/>
       <c r="B22" s="59"/>
       <c r="C22" s="60"/>
@@ -48633,7 +48598,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="14.4" thickBot="1">
+    <row r="32" spans="1:5" ht="14.5" thickBot="1">
       <c r="A32" s="127"/>
       <c r="B32" s="130"/>
       <c r="C32" s="14">
@@ -48646,14 +48611,14 @@
         <v>174</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="14.4" thickBot="1">
+    <row r="33" spans="1:5" ht="14.5" thickBot="1">
       <c r="A33" s="5"/>
       <c r="B33" s="68"/>
       <c r="C33" s="69"/>
       <c r="D33" s="69"/>
       <c r="E33" s="70"/>
     </row>
-    <row r="34" spans="1:5" ht="39.6" customHeight="1">
+    <row r="34" spans="1:5" ht="39.65" customHeight="1">
       <c r="A34" s="107" t="s">
         <v>175</v>
       </c>
@@ -48718,345 +48683,345 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.77734375" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="14.81640625" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="23.5546875" style="40" customWidth="1"/>
-    <col min="2" max="2" width="33.6640625" style="40" customWidth="1"/>
-    <col min="3" max="4" width="14.77734375" style="40" customWidth="1"/>
-    <col min="5" max="5" width="82.44140625" style="40" customWidth="1"/>
-    <col min="6" max="256" width="14.77734375" style="40"/>
-    <col min="257" max="257" width="23.5546875" style="40" customWidth="1"/>
-    <col min="258" max="258" width="33.6640625" style="40" customWidth="1"/>
-    <col min="259" max="260" width="14.77734375" style="40" customWidth="1"/>
-    <col min="261" max="261" width="82.44140625" style="40" customWidth="1"/>
-    <col min="262" max="512" width="14.77734375" style="40"/>
-    <col min="513" max="513" width="23.5546875" style="40" customWidth="1"/>
-    <col min="514" max="514" width="33.6640625" style="40" customWidth="1"/>
-    <col min="515" max="516" width="14.77734375" style="40" customWidth="1"/>
-    <col min="517" max="517" width="82.44140625" style="40" customWidth="1"/>
-    <col min="518" max="768" width="14.77734375" style="40"/>
-    <col min="769" max="769" width="23.5546875" style="40" customWidth="1"/>
-    <col min="770" max="770" width="33.6640625" style="40" customWidth="1"/>
-    <col min="771" max="772" width="14.77734375" style="40" customWidth="1"/>
-    <col min="773" max="773" width="82.44140625" style="40" customWidth="1"/>
-    <col min="774" max="1024" width="14.77734375" style="40"/>
-    <col min="1025" max="1025" width="23.5546875" style="40" customWidth="1"/>
-    <col min="1026" max="1026" width="33.6640625" style="40" customWidth="1"/>
-    <col min="1027" max="1028" width="14.77734375" style="40" customWidth="1"/>
-    <col min="1029" max="1029" width="82.44140625" style="40" customWidth="1"/>
-    <col min="1030" max="1280" width="14.77734375" style="40"/>
-    <col min="1281" max="1281" width="23.5546875" style="40" customWidth="1"/>
-    <col min="1282" max="1282" width="33.6640625" style="40" customWidth="1"/>
-    <col min="1283" max="1284" width="14.77734375" style="40" customWidth="1"/>
-    <col min="1285" max="1285" width="82.44140625" style="40" customWidth="1"/>
-    <col min="1286" max="1536" width="14.77734375" style="40"/>
-    <col min="1537" max="1537" width="23.5546875" style="40" customWidth="1"/>
-    <col min="1538" max="1538" width="33.6640625" style="40" customWidth="1"/>
-    <col min="1539" max="1540" width="14.77734375" style="40" customWidth="1"/>
-    <col min="1541" max="1541" width="82.44140625" style="40" customWidth="1"/>
-    <col min="1542" max="1792" width="14.77734375" style="40"/>
-    <col min="1793" max="1793" width="23.5546875" style="40" customWidth="1"/>
-    <col min="1794" max="1794" width="33.6640625" style="40" customWidth="1"/>
-    <col min="1795" max="1796" width="14.77734375" style="40" customWidth="1"/>
-    <col min="1797" max="1797" width="82.44140625" style="40" customWidth="1"/>
-    <col min="1798" max="2048" width="14.77734375" style="40"/>
-    <col min="2049" max="2049" width="23.5546875" style="40" customWidth="1"/>
-    <col min="2050" max="2050" width="33.6640625" style="40" customWidth="1"/>
-    <col min="2051" max="2052" width="14.77734375" style="40" customWidth="1"/>
-    <col min="2053" max="2053" width="82.44140625" style="40" customWidth="1"/>
-    <col min="2054" max="2304" width="14.77734375" style="40"/>
-    <col min="2305" max="2305" width="23.5546875" style="40" customWidth="1"/>
-    <col min="2306" max="2306" width="33.6640625" style="40" customWidth="1"/>
-    <col min="2307" max="2308" width="14.77734375" style="40" customWidth="1"/>
-    <col min="2309" max="2309" width="82.44140625" style="40" customWidth="1"/>
-    <col min="2310" max="2560" width="14.77734375" style="40"/>
-    <col min="2561" max="2561" width="23.5546875" style="40" customWidth="1"/>
-    <col min="2562" max="2562" width="33.6640625" style="40" customWidth="1"/>
-    <col min="2563" max="2564" width="14.77734375" style="40" customWidth="1"/>
-    <col min="2565" max="2565" width="82.44140625" style="40" customWidth="1"/>
-    <col min="2566" max="2816" width="14.77734375" style="40"/>
-    <col min="2817" max="2817" width="23.5546875" style="40" customWidth="1"/>
-    <col min="2818" max="2818" width="33.6640625" style="40" customWidth="1"/>
-    <col min="2819" max="2820" width="14.77734375" style="40" customWidth="1"/>
-    <col min="2821" max="2821" width="82.44140625" style="40" customWidth="1"/>
-    <col min="2822" max="3072" width="14.77734375" style="40"/>
-    <col min="3073" max="3073" width="23.5546875" style="40" customWidth="1"/>
-    <col min="3074" max="3074" width="33.6640625" style="40" customWidth="1"/>
-    <col min="3075" max="3076" width="14.77734375" style="40" customWidth="1"/>
-    <col min="3077" max="3077" width="82.44140625" style="40" customWidth="1"/>
-    <col min="3078" max="3328" width="14.77734375" style="40"/>
-    <col min="3329" max="3329" width="23.5546875" style="40" customWidth="1"/>
-    <col min="3330" max="3330" width="33.6640625" style="40" customWidth="1"/>
-    <col min="3331" max="3332" width="14.77734375" style="40" customWidth="1"/>
-    <col min="3333" max="3333" width="82.44140625" style="40" customWidth="1"/>
-    <col min="3334" max="3584" width="14.77734375" style="40"/>
-    <col min="3585" max="3585" width="23.5546875" style="40" customWidth="1"/>
-    <col min="3586" max="3586" width="33.6640625" style="40" customWidth="1"/>
-    <col min="3587" max="3588" width="14.77734375" style="40" customWidth="1"/>
-    <col min="3589" max="3589" width="82.44140625" style="40" customWidth="1"/>
-    <col min="3590" max="3840" width="14.77734375" style="40"/>
-    <col min="3841" max="3841" width="23.5546875" style="40" customWidth="1"/>
-    <col min="3842" max="3842" width="33.6640625" style="40" customWidth="1"/>
-    <col min="3843" max="3844" width="14.77734375" style="40" customWidth="1"/>
-    <col min="3845" max="3845" width="82.44140625" style="40" customWidth="1"/>
-    <col min="3846" max="4096" width="14.77734375" style="40"/>
-    <col min="4097" max="4097" width="23.5546875" style="40" customWidth="1"/>
-    <col min="4098" max="4098" width="33.6640625" style="40" customWidth="1"/>
-    <col min="4099" max="4100" width="14.77734375" style="40" customWidth="1"/>
-    <col min="4101" max="4101" width="82.44140625" style="40" customWidth="1"/>
-    <col min="4102" max="4352" width="14.77734375" style="40"/>
-    <col min="4353" max="4353" width="23.5546875" style="40" customWidth="1"/>
-    <col min="4354" max="4354" width="33.6640625" style="40" customWidth="1"/>
-    <col min="4355" max="4356" width="14.77734375" style="40" customWidth="1"/>
-    <col min="4357" max="4357" width="82.44140625" style="40" customWidth="1"/>
-    <col min="4358" max="4608" width="14.77734375" style="40"/>
-    <col min="4609" max="4609" width="23.5546875" style="40" customWidth="1"/>
-    <col min="4610" max="4610" width="33.6640625" style="40" customWidth="1"/>
-    <col min="4611" max="4612" width="14.77734375" style="40" customWidth="1"/>
-    <col min="4613" max="4613" width="82.44140625" style="40" customWidth="1"/>
-    <col min="4614" max="4864" width="14.77734375" style="40"/>
-    <col min="4865" max="4865" width="23.5546875" style="40" customWidth="1"/>
-    <col min="4866" max="4866" width="33.6640625" style="40" customWidth="1"/>
-    <col min="4867" max="4868" width="14.77734375" style="40" customWidth="1"/>
-    <col min="4869" max="4869" width="82.44140625" style="40" customWidth="1"/>
-    <col min="4870" max="5120" width="14.77734375" style="40"/>
-    <col min="5121" max="5121" width="23.5546875" style="40" customWidth="1"/>
-    <col min="5122" max="5122" width="33.6640625" style="40" customWidth="1"/>
-    <col min="5123" max="5124" width="14.77734375" style="40" customWidth="1"/>
-    <col min="5125" max="5125" width="82.44140625" style="40" customWidth="1"/>
-    <col min="5126" max="5376" width="14.77734375" style="40"/>
-    <col min="5377" max="5377" width="23.5546875" style="40" customWidth="1"/>
-    <col min="5378" max="5378" width="33.6640625" style="40" customWidth="1"/>
-    <col min="5379" max="5380" width="14.77734375" style="40" customWidth="1"/>
-    <col min="5381" max="5381" width="82.44140625" style="40" customWidth="1"/>
-    <col min="5382" max="5632" width="14.77734375" style="40"/>
-    <col min="5633" max="5633" width="23.5546875" style="40" customWidth="1"/>
-    <col min="5634" max="5634" width="33.6640625" style="40" customWidth="1"/>
-    <col min="5635" max="5636" width="14.77734375" style="40" customWidth="1"/>
-    <col min="5637" max="5637" width="82.44140625" style="40" customWidth="1"/>
-    <col min="5638" max="5888" width="14.77734375" style="40"/>
-    <col min="5889" max="5889" width="23.5546875" style="40" customWidth="1"/>
-    <col min="5890" max="5890" width="33.6640625" style="40" customWidth="1"/>
-    <col min="5891" max="5892" width="14.77734375" style="40" customWidth="1"/>
-    <col min="5893" max="5893" width="82.44140625" style="40" customWidth="1"/>
-    <col min="5894" max="6144" width="14.77734375" style="40"/>
-    <col min="6145" max="6145" width="23.5546875" style="40" customWidth="1"/>
-    <col min="6146" max="6146" width="33.6640625" style="40" customWidth="1"/>
-    <col min="6147" max="6148" width="14.77734375" style="40" customWidth="1"/>
-    <col min="6149" max="6149" width="82.44140625" style="40" customWidth="1"/>
-    <col min="6150" max="6400" width="14.77734375" style="40"/>
-    <col min="6401" max="6401" width="23.5546875" style="40" customWidth="1"/>
-    <col min="6402" max="6402" width="33.6640625" style="40" customWidth="1"/>
-    <col min="6403" max="6404" width="14.77734375" style="40" customWidth="1"/>
-    <col min="6405" max="6405" width="82.44140625" style="40" customWidth="1"/>
-    <col min="6406" max="6656" width="14.77734375" style="40"/>
-    <col min="6657" max="6657" width="23.5546875" style="40" customWidth="1"/>
-    <col min="6658" max="6658" width="33.6640625" style="40" customWidth="1"/>
-    <col min="6659" max="6660" width="14.77734375" style="40" customWidth="1"/>
-    <col min="6661" max="6661" width="82.44140625" style="40" customWidth="1"/>
-    <col min="6662" max="6912" width="14.77734375" style="40"/>
-    <col min="6913" max="6913" width="23.5546875" style="40" customWidth="1"/>
-    <col min="6914" max="6914" width="33.6640625" style="40" customWidth="1"/>
-    <col min="6915" max="6916" width="14.77734375" style="40" customWidth="1"/>
-    <col min="6917" max="6917" width="82.44140625" style="40" customWidth="1"/>
-    <col min="6918" max="7168" width="14.77734375" style="40"/>
-    <col min="7169" max="7169" width="23.5546875" style="40" customWidth="1"/>
-    <col min="7170" max="7170" width="33.6640625" style="40" customWidth="1"/>
-    <col min="7171" max="7172" width="14.77734375" style="40" customWidth="1"/>
-    <col min="7173" max="7173" width="82.44140625" style="40" customWidth="1"/>
-    <col min="7174" max="7424" width="14.77734375" style="40"/>
-    <col min="7425" max="7425" width="23.5546875" style="40" customWidth="1"/>
-    <col min="7426" max="7426" width="33.6640625" style="40" customWidth="1"/>
-    <col min="7427" max="7428" width="14.77734375" style="40" customWidth="1"/>
-    <col min="7429" max="7429" width="82.44140625" style="40" customWidth="1"/>
-    <col min="7430" max="7680" width="14.77734375" style="40"/>
-    <col min="7681" max="7681" width="23.5546875" style="40" customWidth="1"/>
-    <col min="7682" max="7682" width="33.6640625" style="40" customWidth="1"/>
-    <col min="7683" max="7684" width="14.77734375" style="40" customWidth="1"/>
-    <col min="7685" max="7685" width="82.44140625" style="40" customWidth="1"/>
-    <col min="7686" max="7936" width="14.77734375" style="40"/>
-    <col min="7937" max="7937" width="23.5546875" style="40" customWidth="1"/>
-    <col min="7938" max="7938" width="33.6640625" style="40" customWidth="1"/>
-    <col min="7939" max="7940" width="14.77734375" style="40" customWidth="1"/>
-    <col min="7941" max="7941" width="82.44140625" style="40" customWidth="1"/>
-    <col min="7942" max="8192" width="14.77734375" style="40"/>
-    <col min="8193" max="8193" width="23.5546875" style="40" customWidth="1"/>
-    <col min="8194" max="8194" width="33.6640625" style="40" customWidth="1"/>
-    <col min="8195" max="8196" width="14.77734375" style="40" customWidth="1"/>
-    <col min="8197" max="8197" width="82.44140625" style="40" customWidth="1"/>
-    <col min="8198" max="8448" width="14.77734375" style="40"/>
-    <col min="8449" max="8449" width="23.5546875" style="40" customWidth="1"/>
-    <col min="8450" max="8450" width="33.6640625" style="40" customWidth="1"/>
-    <col min="8451" max="8452" width="14.77734375" style="40" customWidth="1"/>
-    <col min="8453" max="8453" width="82.44140625" style="40" customWidth="1"/>
-    <col min="8454" max="8704" width="14.77734375" style="40"/>
-    <col min="8705" max="8705" width="23.5546875" style="40" customWidth="1"/>
-    <col min="8706" max="8706" width="33.6640625" style="40" customWidth="1"/>
-    <col min="8707" max="8708" width="14.77734375" style="40" customWidth="1"/>
-    <col min="8709" max="8709" width="82.44140625" style="40" customWidth="1"/>
-    <col min="8710" max="8960" width="14.77734375" style="40"/>
-    <col min="8961" max="8961" width="23.5546875" style="40" customWidth="1"/>
-    <col min="8962" max="8962" width="33.6640625" style="40" customWidth="1"/>
-    <col min="8963" max="8964" width="14.77734375" style="40" customWidth="1"/>
-    <col min="8965" max="8965" width="82.44140625" style="40" customWidth="1"/>
-    <col min="8966" max="9216" width="14.77734375" style="40"/>
-    <col min="9217" max="9217" width="23.5546875" style="40" customWidth="1"/>
-    <col min="9218" max="9218" width="33.6640625" style="40" customWidth="1"/>
-    <col min="9219" max="9220" width="14.77734375" style="40" customWidth="1"/>
-    <col min="9221" max="9221" width="82.44140625" style="40" customWidth="1"/>
-    <col min="9222" max="9472" width="14.77734375" style="40"/>
-    <col min="9473" max="9473" width="23.5546875" style="40" customWidth="1"/>
-    <col min="9474" max="9474" width="33.6640625" style="40" customWidth="1"/>
-    <col min="9475" max="9476" width="14.77734375" style="40" customWidth="1"/>
-    <col min="9477" max="9477" width="82.44140625" style="40" customWidth="1"/>
-    <col min="9478" max="9728" width="14.77734375" style="40"/>
-    <col min="9729" max="9729" width="23.5546875" style="40" customWidth="1"/>
-    <col min="9730" max="9730" width="33.6640625" style="40" customWidth="1"/>
-    <col min="9731" max="9732" width="14.77734375" style="40" customWidth="1"/>
-    <col min="9733" max="9733" width="82.44140625" style="40" customWidth="1"/>
-    <col min="9734" max="9984" width="14.77734375" style="40"/>
-    <col min="9985" max="9985" width="23.5546875" style="40" customWidth="1"/>
-    <col min="9986" max="9986" width="33.6640625" style="40" customWidth="1"/>
-    <col min="9987" max="9988" width="14.77734375" style="40" customWidth="1"/>
-    <col min="9989" max="9989" width="82.44140625" style="40" customWidth="1"/>
-    <col min="9990" max="10240" width="14.77734375" style="40"/>
-    <col min="10241" max="10241" width="23.5546875" style="40" customWidth="1"/>
-    <col min="10242" max="10242" width="33.6640625" style="40" customWidth="1"/>
-    <col min="10243" max="10244" width="14.77734375" style="40" customWidth="1"/>
-    <col min="10245" max="10245" width="82.44140625" style="40" customWidth="1"/>
-    <col min="10246" max="10496" width="14.77734375" style="40"/>
-    <col min="10497" max="10497" width="23.5546875" style="40" customWidth="1"/>
-    <col min="10498" max="10498" width="33.6640625" style="40" customWidth="1"/>
-    <col min="10499" max="10500" width="14.77734375" style="40" customWidth="1"/>
-    <col min="10501" max="10501" width="82.44140625" style="40" customWidth="1"/>
-    <col min="10502" max="10752" width="14.77734375" style="40"/>
-    <col min="10753" max="10753" width="23.5546875" style="40" customWidth="1"/>
-    <col min="10754" max="10754" width="33.6640625" style="40" customWidth="1"/>
-    <col min="10755" max="10756" width="14.77734375" style="40" customWidth="1"/>
-    <col min="10757" max="10757" width="82.44140625" style="40" customWidth="1"/>
-    <col min="10758" max="11008" width="14.77734375" style="40"/>
-    <col min="11009" max="11009" width="23.5546875" style="40" customWidth="1"/>
-    <col min="11010" max="11010" width="33.6640625" style="40" customWidth="1"/>
-    <col min="11011" max="11012" width="14.77734375" style="40" customWidth="1"/>
-    <col min="11013" max="11013" width="82.44140625" style="40" customWidth="1"/>
-    <col min="11014" max="11264" width="14.77734375" style="40"/>
-    <col min="11265" max="11265" width="23.5546875" style="40" customWidth="1"/>
-    <col min="11266" max="11266" width="33.6640625" style="40" customWidth="1"/>
-    <col min="11267" max="11268" width="14.77734375" style="40" customWidth="1"/>
-    <col min="11269" max="11269" width="82.44140625" style="40" customWidth="1"/>
-    <col min="11270" max="11520" width="14.77734375" style="40"/>
-    <col min="11521" max="11521" width="23.5546875" style="40" customWidth="1"/>
-    <col min="11522" max="11522" width="33.6640625" style="40" customWidth="1"/>
-    <col min="11523" max="11524" width="14.77734375" style="40" customWidth="1"/>
-    <col min="11525" max="11525" width="82.44140625" style="40" customWidth="1"/>
-    <col min="11526" max="11776" width="14.77734375" style="40"/>
-    <col min="11777" max="11777" width="23.5546875" style="40" customWidth="1"/>
-    <col min="11778" max="11778" width="33.6640625" style="40" customWidth="1"/>
-    <col min="11779" max="11780" width="14.77734375" style="40" customWidth="1"/>
-    <col min="11781" max="11781" width="82.44140625" style="40" customWidth="1"/>
-    <col min="11782" max="12032" width="14.77734375" style="40"/>
-    <col min="12033" max="12033" width="23.5546875" style="40" customWidth="1"/>
-    <col min="12034" max="12034" width="33.6640625" style="40" customWidth="1"/>
-    <col min="12035" max="12036" width="14.77734375" style="40" customWidth="1"/>
-    <col min="12037" max="12037" width="82.44140625" style="40" customWidth="1"/>
-    <col min="12038" max="12288" width="14.77734375" style="40"/>
-    <col min="12289" max="12289" width="23.5546875" style="40" customWidth="1"/>
-    <col min="12290" max="12290" width="33.6640625" style="40" customWidth="1"/>
-    <col min="12291" max="12292" width="14.77734375" style="40" customWidth="1"/>
-    <col min="12293" max="12293" width="82.44140625" style="40" customWidth="1"/>
-    <col min="12294" max="12544" width="14.77734375" style="40"/>
-    <col min="12545" max="12545" width="23.5546875" style="40" customWidth="1"/>
-    <col min="12546" max="12546" width="33.6640625" style="40" customWidth="1"/>
-    <col min="12547" max="12548" width="14.77734375" style="40" customWidth="1"/>
-    <col min="12549" max="12549" width="82.44140625" style="40" customWidth="1"/>
-    <col min="12550" max="12800" width="14.77734375" style="40"/>
-    <col min="12801" max="12801" width="23.5546875" style="40" customWidth="1"/>
-    <col min="12802" max="12802" width="33.6640625" style="40" customWidth="1"/>
-    <col min="12803" max="12804" width="14.77734375" style="40" customWidth="1"/>
-    <col min="12805" max="12805" width="82.44140625" style="40" customWidth="1"/>
-    <col min="12806" max="13056" width="14.77734375" style="40"/>
-    <col min="13057" max="13057" width="23.5546875" style="40" customWidth="1"/>
-    <col min="13058" max="13058" width="33.6640625" style="40" customWidth="1"/>
-    <col min="13059" max="13060" width="14.77734375" style="40" customWidth="1"/>
-    <col min="13061" max="13061" width="82.44140625" style="40" customWidth="1"/>
-    <col min="13062" max="13312" width="14.77734375" style="40"/>
-    <col min="13313" max="13313" width="23.5546875" style="40" customWidth="1"/>
-    <col min="13314" max="13314" width="33.6640625" style="40" customWidth="1"/>
-    <col min="13315" max="13316" width="14.77734375" style="40" customWidth="1"/>
-    <col min="13317" max="13317" width="82.44140625" style="40" customWidth="1"/>
-    <col min="13318" max="13568" width="14.77734375" style="40"/>
-    <col min="13569" max="13569" width="23.5546875" style="40" customWidth="1"/>
-    <col min="13570" max="13570" width="33.6640625" style="40" customWidth="1"/>
-    <col min="13571" max="13572" width="14.77734375" style="40" customWidth="1"/>
-    <col min="13573" max="13573" width="82.44140625" style="40" customWidth="1"/>
-    <col min="13574" max="13824" width="14.77734375" style="40"/>
-    <col min="13825" max="13825" width="23.5546875" style="40" customWidth="1"/>
-    <col min="13826" max="13826" width="33.6640625" style="40" customWidth="1"/>
-    <col min="13827" max="13828" width="14.77734375" style="40" customWidth="1"/>
-    <col min="13829" max="13829" width="82.44140625" style="40" customWidth="1"/>
-    <col min="13830" max="14080" width="14.77734375" style="40"/>
-    <col min="14081" max="14081" width="23.5546875" style="40" customWidth="1"/>
-    <col min="14082" max="14082" width="33.6640625" style="40" customWidth="1"/>
-    <col min="14083" max="14084" width="14.77734375" style="40" customWidth="1"/>
-    <col min="14085" max="14085" width="82.44140625" style="40" customWidth="1"/>
-    <col min="14086" max="14336" width="14.77734375" style="40"/>
-    <col min="14337" max="14337" width="23.5546875" style="40" customWidth="1"/>
-    <col min="14338" max="14338" width="33.6640625" style="40" customWidth="1"/>
-    <col min="14339" max="14340" width="14.77734375" style="40" customWidth="1"/>
-    <col min="14341" max="14341" width="82.44140625" style="40" customWidth="1"/>
-    <col min="14342" max="14592" width="14.77734375" style="40"/>
-    <col min="14593" max="14593" width="23.5546875" style="40" customWidth="1"/>
-    <col min="14594" max="14594" width="33.6640625" style="40" customWidth="1"/>
-    <col min="14595" max="14596" width="14.77734375" style="40" customWidth="1"/>
-    <col min="14597" max="14597" width="82.44140625" style="40" customWidth="1"/>
-    <col min="14598" max="14848" width="14.77734375" style="40"/>
-    <col min="14849" max="14849" width="23.5546875" style="40" customWidth="1"/>
-    <col min="14850" max="14850" width="33.6640625" style="40" customWidth="1"/>
-    <col min="14851" max="14852" width="14.77734375" style="40" customWidth="1"/>
-    <col min="14853" max="14853" width="82.44140625" style="40" customWidth="1"/>
-    <col min="14854" max="15104" width="14.77734375" style="40"/>
-    <col min="15105" max="15105" width="23.5546875" style="40" customWidth="1"/>
-    <col min="15106" max="15106" width="33.6640625" style="40" customWidth="1"/>
-    <col min="15107" max="15108" width="14.77734375" style="40" customWidth="1"/>
-    <col min="15109" max="15109" width="82.44140625" style="40" customWidth="1"/>
-    <col min="15110" max="15360" width="14.77734375" style="40"/>
-    <col min="15361" max="15361" width="23.5546875" style="40" customWidth="1"/>
-    <col min="15362" max="15362" width="33.6640625" style="40" customWidth="1"/>
-    <col min="15363" max="15364" width="14.77734375" style="40" customWidth="1"/>
-    <col min="15365" max="15365" width="82.44140625" style="40" customWidth="1"/>
-    <col min="15366" max="15616" width="14.77734375" style="40"/>
-    <col min="15617" max="15617" width="23.5546875" style="40" customWidth="1"/>
-    <col min="15618" max="15618" width="33.6640625" style="40" customWidth="1"/>
-    <col min="15619" max="15620" width="14.77734375" style="40" customWidth="1"/>
-    <col min="15621" max="15621" width="82.44140625" style="40" customWidth="1"/>
-    <col min="15622" max="15872" width="14.77734375" style="40"/>
-    <col min="15873" max="15873" width="23.5546875" style="40" customWidth="1"/>
-    <col min="15874" max="15874" width="33.6640625" style="40" customWidth="1"/>
-    <col min="15875" max="15876" width="14.77734375" style="40" customWidth="1"/>
-    <col min="15877" max="15877" width="82.44140625" style="40" customWidth="1"/>
-    <col min="15878" max="16128" width="14.77734375" style="40"/>
-    <col min="16129" max="16129" width="23.5546875" style="40" customWidth="1"/>
-    <col min="16130" max="16130" width="33.6640625" style="40" customWidth="1"/>
-    <col min="16131" max="16132" width="14.77734375" style="40" customWidth="1"/>
-    <col min="16133" max="16133" width="82.44140625" style="40" customWidth="1"/>
-    <col min="16134" max="16384" width="14.77734375" style="40"/>
+    <col min="1" max="1" width="23.54296875" style="40" customWidth="1"/>
+    <col min="2" max="2" width="33.6328125" style="40" customWidth="1"/>
+    <col min="3" max="4" width="14.81640625" style="40" customWidth="1"/>
+    <col min="5" max="5" width="82.453125" style="40" customWidth="1"/>
+    <col min="6" max="256" width="14.81640625" style="40"/>
+    <col min="257" max="257" width="23.54296875" style="40" customWidth="1"/>
+    <col min="258" max="258" width="33.6328125" style="40" customWidth="1"/>
+    <col min="259" max="260" width="14.81640625" style="40" customWidth="1"/>
+    <col min="261" max="261" width="82.453125" style="40" customWidth="1"/>
+    <col min="262" max="512" width="14.81640625" style="40"/>
+    <col min="513" max="513" width="23.54296875" style="40" customWidth="1"/>
+    <col min="514" max="514" width="33.6328125" style="40" customWidth="1"/>
+    <col min="515" max="516" width="14.81640625" style="40" customWidth="1"/>
+    <col min="517" max="517" width="82.453125" style="40" customWidth="1"/>
+    <col min="518" max="768" width="14.81640625" style="40"/>
+    <col min="769" max="769" width="23.54296875" style="40" customWidth="1"/>
+    <col min="770" max="770" width="33.6328125" style="40" customWidth="1"/>
+    <col min="771" max="772" width="14.81640625" style="40" customWidth="1"/>
+    <col min="773" max="773" width="82.453125" style="40" customWidth="1"/>
+    <col min="774" max="1024" width="14.81640625" style="40"/>
+    <col min="1025" max="1025" width="23.54296875" style="40" customWidth="1"/>
+    <col min="1026" max="1026" width="33.6328125" style="40" customWidth="1"/>
+    <col min="1027" max="1028" width="14.81640625" style="40" customWidth="1"/>
+    <col min="1029" max="1029" width="82.453125" style="40" customWidth="1"/>
+    <col min="1030" max="1280" width="14.81640625" style="40"/>
+    <col min="1281" max="1281" width="23.54296875" style="40" customWidth="1"/>
+    <col min="1282" max="1282" width="33.6328125" style="40" customWidth="1"/>
+    <col min="1283" max="1284" width="14.81640625" style="40" customWidth="1"/>
+    <col min="1285" max="1285" width="82.453125" style="40" customWidth="1"/>
+    <col min="1286" max="1536" width="14.81640625" style="40"/>
+    <col min="1537" max="1537" width="23.54296875" style="40" customWidth="1"/>
+    <col min="1538" max="1538" width="33.6328125" style="40" customWidth="1"/>
+    <col min="1539" max="1540" width="14.81640625" style="40" customWidth="1"/>
+    <col min="1541" max="1541" width="82.453125" style="40" customWidth="1"/>
+    <col min="1542" max="1792" width="14.81640625" style="40"/>
+    <col min="1793" max="1793" width="23.54296875" style="40" customWidth="1"/>
+    <col min="1794" max="1794" width="33.6328125" style="40" customWidth="1"/>
+    <col min="1795" max="1796" width="14.81640625" style="40" customWidth="1"/>
+    <col min="1797" max="1797" width="82.453125" style="40" customWidth="1"/>
+    <col min="1798" max="2048" width="14.81640625" style="40"/>
+    <col min="2049" max="2049" width="23.54296875" style="40" customWidth="1"/>
+    <col min="2050" max="2050" width="33.6328125" style="40" customWidth="1"/>
+    <col min="2051" max="2052" width="14.81640625" style="40" customWidth="1"/>
+    <col min="2053" max="2053" width="82.453125" style="40" customWidth="1"/>
+    <col min="2054" max="2304" width="14.81640625" style="40"/>
+    <col min="2305" max="2305" width="23.54296875" style="40" customWidth="1"/>
+    <col min="2306" max="2306" width="33.6328125" style="40" customWidth="1"/>
+    <col min="2307" max="2308" width="14.81640625" style="40" customWidth="1"/>
+    <col min="2309" max="2309" width="82.453125" style="40" customWidth="1"/>
+    <col min="2310" max="2560" width="14.81640625" style="40"/>
+    <col min="2561" max="2561" width="23.54296875" style="40" customWidth="1"/>
+    <col min="2562" max="2562" width="33.6328125" style="40" customWidth="1"/>
+    <col min="2563" max="2564" width="14.81640625" style="40" customWidth="1"/>
+    <col min="2565" max="2565" width="82.453125" style="40" customWidth="1"/>
+    <col min="2566" max="2816" width="14.81640625" style="40"/>
+    <col min="2817" max="2817" width="23.54296875" style="40" customWidth="1"/>
+    <col min="2818" max="2818" width="33.6328125" style="40" customWidth="1"/>
+    <col min="2819" max="2820" width="14.81640625" style="40" customWidth="1"/>
+    <col min="2821" max="2821" width="82.453125" style="40" customWidth="1"/>
+    <col min="2822" max="3072" width="14.81640625" style="40"/>
+    <col min="3073" max="3073" width="23.54296875" style="40" customWidth="1"/>
+    <col min="3074" max="3074" width="33.6328125" style="40" customWidth="1"/>
+    <col min="3075" max="3076" width="14.81640625" style="40" customWidth="1"/>
+    <col min="3077" max="3077" width="82.453125" style="40" customWidth="1"/>
+    <col min="3078" max="3328" width="14.81640625" style="40"/>
+    <col min="3329" max="3329" width="23.54296875" style="40" customWidth="1"/>
+    <col min="3330" max="3330" width="33.6328125" style="40" customWidth="1"/>
+    <col min="3331" max="3332" width="14.81640625" style="40" customWidth="1"/>
+    <col min="3333" max="3333" width="82.453125" style="40" customWidth="1"/>
+    <col min="3334" max="3584" width="14.81640625" style="40"/>
+    <col min="3585" max="3585" width="23.54296875" style="40" customWidth="1"/>
+    <col min="3586" max="3586" width="33.6328125" style="40" customWidth="1"/>
+    <col min="3587" max="3588" width="14.81640625" style="40" customWidth="1"/>
+    <col min="3589" max="3589" width="82.453125" style="40" customWidth="1"/>
+    <col min="3590" max="3840" width="14.81640625" style="40"/>
+    <col min="3841" max="3841" width="23.54296875" style="40" customWidth="1"/>
+    <col min="3842" max="3842" width="33.6328125" style="40" customWidth="1"/>
+    <col min="3843" max="3844" width="14.81640625" style="40" customWidth="1"/>
+    <col min="3845" max="3845" width="82.453125" style="40" customWidth="1"/>
+    <col min="3846" max="4096" width="14.81640625" style="40"/>
+    <col min="4097" max="4097" width="23.54296875" style="40" customWidth="1"/>
+    <col min="4098" max="4098" width="33.6328125" style="40" customWidth="1"/>
+    <col min="4099" max="4100" width="14.81640625" style="40" customWidth="1"/>
+    <col min="4101" max="4101" width="82.453125" style="40" customWidth="1"/>
+    <col min="4102" max="4352" width="14.81640625" style="40"/>
+    <col min="4353" max="4353" width="23.54296875" style="40" customWidth="1"/>
+    <col min="4354" max="4354" width="33.6328125" style="40" customWidth="1"/>
+    <col min="4355" max="4356" width="14.81640625" style="40" customWidth="1"/>
+    <col min="4357" max="4357" width="82.453125" style="40" customWidth="1"/>
+    <col min="4358" max="4608" width="14.81640625" style="40"/>
+    <col min="4609" max="4609" width="23.54296875" style="40" customWidth="1"/>
+    <col min="4610" max="4610" width="33.6328125" style="40" customWidth="1"/>
+    <col min="4611" max="4612" width="14.81640625" style="40" customWidth="1"/>
+    <col min="4613" max="4613" width="82.453125" style="40" customWidth="1"/>
+    <col min="4614" max="4864" width="14.81640625" style="40"/>
+    <col min="4865" max="4865" width="23.54296875" style="40" customWidth="1"/>
+    <col min="4866" max="4866" width="33.6328125" style="40" customWidth="1"/>
+    <col min="4867" max="4868" width="14.81640625" style="40" customWidth="1"/>
+    <col min="4869" max="4869" width="82.453125" style="40" customWidth="1"/>
+    <col min="4870" max="5120" width="14.81640625" style="40"/>
+    <col min="5121" max="5121" width="23.54296875" style="40" customWidth="1"/>
+    <col min="5122" max="5122" width="33.6328125" style="40" customWidth="1"/>
+    <col min="5123" max="5124" width="14.81640625" style="40" customWidth="1"/>
+    <col min="5125" max="5125" width="82.453125" style="40" customWidth="1"/>
+    <col min="5126" max="5376" width="14.81640625" style="40"/>
+    <col min="5377" max="5377" width="23.54296875" style="40" customWidth="1"/>
+    <col min="5378" max="5378" width="33.6328125" style="40" customWidth="1"/>
+    <col min="5379" max="5380" width="14.81640625" style="40" customWidth="1"/>
+    <col min="5381" max="5381" width="82.453125" style="40" customWidth="1"/>
+    <col min="5382" max="5632" width="14.81640625" style="40"/>
+    <col min="5633" max="5633" width="23.54296875" style="40" customWidth="1"/>
+    <col min="5634" max="5634" width="33.6328125" style="40" customWidth="1"/>
+    <col min="5635" max="5636" width="14.81640625" style="40" customWidth="1"/>
+    <col min="5637" max="5637" width="82.453125" style="40" customWidth="1"/>
+    <col min="5638" max="5888" width="14.81640625" style="40"/>
+    <col min="5889" max="5889" width="23.54296875" style="40" customWidth="1"/>
+    <col min="5890" max="5890" width="33.6328125" style="40" customWidth="1"/>
+    <col min="5891" max="5892" width="14.81640625" style="40" customWidth="1"/>
+    <col min="5893" max="5893" width="82.453125" style="40" customWidth="1"/>
+    <col min="5894" max="6144" width="14.81640625" style="40"/>
+    <col min="6145" max="6145" width="23.54296875" style="40" customWidth="1"/>
+    <col min="6146" max="6146" width="33.6328125" style="40" customWidth="1"/>
+    <col min="6147" max="6148" width="14.81640625" style="40" customWidth="1"/>
+    <col min="6149" max="6149" width="82.453125" style="40" customWidth="1"/>
+    <col min="6150" max="6400" width="14.81640625" style="40"/>
+    <col min="6401" max="6401" width="23.54296875" style="40" customWidth="1"/>
+    <col min="6402" max="6402" width="33.6328125" style="40" customWidth="1"/>
+    <col min="6403" max="6404" width="14.81640625" style="40" customWidth="1"/>
+    <col min="6405" max="6405" width="82.453125" style="40" customWidth="1"/>
+    <col min="6406" max="6656" width="14.81640625" style="40"/>
+    <col min="6657" max="6657" width="23.54296875" style="40" customWidth="1"/>
+    <col min="6658" max="6658" width="33.6328125" style="40" customWidth="1"/>
+    <col min="6659" max="6660" width="14.81640625" style="40" customWidth="1"/>
+    <col min="6661" max="6661" width="82.453125" style="40" customWidth="1"/>
+    <col min="6662" max="6912" width="14.81640625" style="40"/>
+    <col min="6913" max="6913" width="23.54296875" style="40" customWidth="1"/>
+    <col min="6914" max="6914" width="33.6328125" style="40" customWidth="1"/>
+    <col min="6915" max="6916" width="14.81640625" style="40" customWidth="1"/>
+    <col min="6917" max="6917" width="82.453125" style="40" customWidth="1"/>
+    <col min="6918" max="7168" width="14.81640625" style="40"/>
+    <col min="7169" max="7169" width="23.54296875" style="40" customWidth="1"/>
+    <col min="7170" max="7170" width="33.6328125" style="40" customWidth="1"/>
+    <col min="7171" max="7172" width="14.81640625" style="40" customWidth="1"/>
+    <col min="7173" max="7173" width="82.453125" style="40" customWidth="1"/>
+    <col min="7174" max="7424" width="14.81640625" style="40"/>
+    <col min="7425" max="7425" width="23.54296875" style="40" customWidth="1"/>
+    <col min="7426" max="7426" width="33.6328125" style="40" customWidth="1"/>
+    <col min="7427" max="7428" width="14.81640625" style="40" customWidth="1"/>
+    <col min="7429" max="7429" width="82.453125" style="40" customWidth="1"/>
+    <col min="7430" max="7680" width="14.81640625" style="40"/>
+    <col min="7681" max="7681" width="23.54296875" style="40" customWidth="1"/>
+    <col min="7682" max="7682" width="33.6328125" style="40" customWidth="1"/>
+    <col min="7683" max="7684" width="14.81640625" style="40" customWidth="1"/>
+    <col min="7685" max="7685" width="82.453125" style="40" customWidth="1"/>
+    <col min="7686" max="7936" width="14.81640625" style="40"/>
+    <col min="7937" max="7937" width="23.54296875" style="40" customWidth="1"/>
+    <col min="7938" max="7938" width="33.6328125" style="40" customWidth="1"/>
+    <col min="7939" max="7940" width="14.81640625" style="40" customWidth="1"/>
+    <col min="7941" max="7941" width="82.453125" style="40" customWidth="1"/>
+    <col min="7942" max="8192" width="14.81640625" style="40"/>
+    <col min="8193" max="8193" width="23.54296875" style="40" customWidth="1"/>
+    <col min="8194" max="8194" width="33.6328125" style="40" customWidth="1"/>
+    <col min="8195" max="8196" width="14.81640625" style="40" customWidth="1"/>
+    <col min="8197" max="8197" width="82.453125" style="40" customWidth="1"/>
+    <col min="8198" max="8448" width="14.81640625" style="40"/>
+    <col min="8449" max="8449" width="23.54296875" style="40" customWidth="1"/>
+    <col min="8450" max="8450" width="33.6328125" style="40" customWidth="1"/>
+    <col min="8451" max="8452" width="14.81640625" style="40" customWidth="1"/>
+    <col min="8453" max="8453" width="82.453125" style="40" customWidth="1"/>
+    <col min="8454" max="8704" width="14.81640625" style="40"/>
+    <col min="8705" max="8705" width="23.54296875" style="40" customWidth="1"/>
+    <col min="8706" max="8706" width="33.6328125" style="40" customWidth="1"/>
+    <col min="8707" max="8708" width="14.81640625" style="40" customWidth="1"/>
+    <col min="8709" max="8709" width="82.453125" style="40" customWidth="1"/>
+    <col min="8710" max="8960" width="14.81640625" style="40"/>
+    <col min="8961" max="8961" width="23.54296875" style="40" customWidth="1"/>
+    <col min="8962" max="8962" width="33.6328125" style="40" customWidth="1"/>
+    <col min="8963" max="8964" width="14.81640625" style="40" customWidth="1"/>
+    <col min="8965" max="8965" width="82.453125" style="40" customWidth="1"/>
+    <col min="8966" max="9216" width="14.81640625" style="40"/>
+    <col min="9217" max="9217" width="23.54296875" style="40" customWidth="1"/>
+    <col min="9218" max="9218" width="33.6328125" style="40" customWidth="1"/>
+    <col min="9219" max="9220" width="14.81640625" style="40" customWidth="1"/>
+    <col min="9221" max="9221" width="82.453125" style="40" customWidth="1"/>
+    <col min="9222" max="9472" width="14.81640625" style="40"/>
+    <col min="9473" max="9473" width="23.54296875" style="40" customWidth="1"/>
+    <col min="9474" max="9474" width="33.6328125" style="40" customWidth="1"/>
+    <col min="9475" max="9476" width="14.81640625" style="40" customWidth="1"/>
+    <col min="9477" max="9477" width="82.453125" style="40" customWidth="1"/>
+    <col min="9478" max="9728" width="14.81640625" style="40"/>
+    <col min="9729" max="9729" width="23.54296875" style="40" customWidth="1"/>
+    <col min="9730" max="9730" width="33.6328125" style="40" customWidth="1"/>
+    <col min="9731" max="9732" width="14.81640625" style="40" customWidth="1"/>
+    <col min="9733" max="9733" width="82.453125" style="40" customWidth="1"/>
+    <col min="9734" max="9984" width="14.81640625" style="40"/>
+    <col min="9985" max="9985" width="23.54296875" style="40" customWidth="1"/>
+    <col min="9986" max="9986" width="33.6328125" style="40" customWidth="1"/>
+    <col min="9987" max="9988" width="14.81640625" style="40" customWidth="1"/>
+    <col min="9989" max="9989" width="82.453125" style="40" customWidth="1"/>
+    <col min="9990" max="10240" width="14.81640625" style="40"/>
+    <col min="10241" max="10241" width="23.54296875" style="40" customWidth="1"/>
+    <col min="10242" max="10242" width="33.6328125" style="40" customWidth="1"/>
+    <col min="10243" max="10244" width="14.81640625" style="40" customWidth="1"/>
+    <col min="10245" max="10245" width="82.453125" style="40" customWidth="1"/>
+    <col min="10246" max="10496" width="14.81640625" style="40"/>
+    <col min="10497" max="10497" width="23.54296875" style="40" customWidth="1"/>
+    <col min="10498" max="10498" width="33.6328125" style="40" customWidth="1"/>
+    <col min="10499" max="10500" width="14.81640625" style="40" customWidth="1"/>
+    <col min="10501" max="10501" width="82.453125" style="40" customWidth="1"/>
+    <col min="10502" max="10752" width="14.81640625" style="40"/>
+    <col min="10753" max="10753" width="23.54296875" style="40" customWidth="1"/>
+    <col min="10754" max="10754" width="33.6328125" style="40" customWidth="1"/>
+    <col min="10755" max="10756" width="14.81640625" style="40" customWidth="1"/>
+    <col min="10757" max="10757" width="82.453125" style="40" customWidth="1"/>
+    <col min="10758" max="11008" width="14.81640625" style="40"/>
+    <col min="11009" max="11009" width="23.54296875" style="40" customWidth="1"/>
+    <col min="11010" max="11010" width="33.6328125" style="40" customWidth="1"/>
+    <col min="11011" max="11012" width="14.81640625" style="40" customWidth="1"/>
+    <col min="11013" max="11013" width="82.453125" style="40" customWidth="1"/>
+    <col min="11014" max="11264" width="14.81640625" style="40"/>
+    <col min="11265" max="11265" width="23.54296875" style="40" customWidth="1"/>
+    <col min="11266" max="11266" width="33.6328125" style="40" customWidth="1"/>
+    <col min="11267" max="11268" width="14.81640625" style="40" customWidth="1"/>
+    <col min="11269" max="11269" width="82.453125" style="40" customWidth="1"/>
+    <col min="11270" max="11520" width="14.81640625" style="40"/>
+    <col min="11521" max="11521" width="23.54296875" style="40" customWidth="1"/>
+    <col min="11522" max="11522" width="33.6328125" style="40" customWidth="1"/>
+    <col min="11523" max="11524" width="14.81640625" style="40" customWidth="1"/>
+    <col min="11525" max="11525" width="82.453125" style="40" customWidth="1"/>
+    <col min="11526" max="11776" width="14.81640625" style="40"/>
+    <col min="11777" max="11777" width="23.54296875" style="40" customWidth="1"/>
+    <col min="11778" max="11778" width="33.6328125" style="40" customWidth="1"/>
+    <col min="11779" max="11780" width="14.81640625" style="40" customWidth="1"/>
+    <col min="11781" max="11781" width="82.453125" style="40" customWidth="1"/>
+    <col min="11782" max="12032" width="14.81640625" style="40"/>
+    <col min="12033" max="12033" width="23.54296875" style="40" customWidth="1"/>
+    <col min="12034" max="12034" width="33.6328125" style="40" customWidth="1"/>
+    <col min="12035" max="12036" width="14.81640625" style="40" customWidth="1"/>
+    <col min="12037" max="12037" width="82.453125" style="40" customWidth="1"/>
+    <col min="12038" max="12288" width="14.81640625" style="40"/>
+    <col min="12289" max="12289" width="23.54296875" style="40" customWidth="1"/>
+    <col min="12290" max="12290" width="33.6328125" style="40" customWidth="1"/>
+    <col min="12291" max="12292" width="14.81640625" style="40" customWidth="1"/>
+    <col min="12293" max="12293" width="82.453125" style="40" customWidth="1"/>
+    <col min="12294" max="12544" width="14.81640625" style="40"/>
+    <col min="12545" max="12545" width="23.54296875" style="40" customWidth="1"/>
+    <col min="12546" max="12546" width="33.6328125" style="40" customWidth="1"/>
+    <col min="12547" max="12548" width="14.81640625" style="40" customWidth="1"/>
+    <col min="12549" max="12549" width="82.453125" style="40" customWidth="1"/>
+    <col min="12550" max="12800" width="14.81640625" style="40"/>
+    <col min="12801" max="12801" width="23.54296875" style="40" customWidth="1"/>
+    <col min="12802" max="12802" width="33.6328125" style="40" customWidth="1"/>
+    <col min="12803" max="12804" width="14.81640625" style="40" customWidth="1"/>
+    <col min="12805" max="12805" width="82.453125" style="40" customWidth="1"/>
+    <col min="12806" max="13056" width="14.81640625" style="40"/>
+    <col min="13057" max="13057" width="23.54296875" style="40" customWidth="1"/>
+    <col min="13058" max="13058" width="33.6328125" style="40" customWidth="1"/>
+    <col min="13059" max="13060" width="14.81640625" style="40" customWidth="1"/>
+    <col min="13061" max="13061" width="82.453125" style="40" customWidth="1"/>
+    <col min="13062" max="13312" width="14.81640625" style="40"/>
+    <col min="13313" max="13313" width="23.54296875" style="40" customWidth="1"/>
+    <col min="13314" max="13314" width="33.6328125" style="40" customWidth="1"/>
+    <col min="13315" max="13316" width="14.81640625" style="40" customWidth="1"/>
+    <col min="13317" max="13317" width="82.453125" style="40" customWidth="1"/>
+    <col min="13318" max="13568" width="14.81640625" style="40"/>
+    <col min="13569" max="13569" width="23.54296875" style="40" customWidth="1"/>
+    <col min="13570" max="13570" width="33.6328125" style="40" customWidth="1"/>
+    <col min="13571" max="13572" width="14.81640625" style="40" customWidth="1"/>
+    <col min="13573" max="13573" width="82.453125" style="40" customWidth="1"/>
+    <col min="13574" max="13824" width="14.81640625" style="40"/>
+    <col min="13825" max="13825" width="23.54296875" style="40" customWidth="1"/>
+    <col min="13826" max="13826" width="33.6328125" style="40" customWidth="1"/>
+    <col min="13827" max="13828" width="14.81640625" style="40" customWidth="1"/>
+    <col min="13829" max="13829" width="82.453125" style="40" customWidth="1"/>
+    <col min="13830" max="14080" width="14.81640625" style="40"/>
+    <col min="14081" max="14081" width="23.54296875" style="40" customWidth="1"/>
+    <col min="14082" max="14082" width="33.6328125" style="40" customWidth="1"/>
+    <col min="14083" max="14084" width="14.81640625" style="40" customWidth="1"/>
+    <col min="14085" max="14085" width="82.453125" style="40" customWidth="1"/>
+    <col min="14086" max="14336" width="14.81640625" style="40"/>
+    <col min="14337" max="14337" width="23.54296875" style="40" customWidth="1"/>
+    <col min="14338" max="14338" width="33.6328125" style="40" customWidth="1"/>
+    <col min="14339" max="14340" width="14.81640625" style="40" customWidth="1"/>
+    <col min="14341" max="14341" width="82.453125" style="40" customWidth="1"/>
+    <col min="14342" max="14592" width="14.81640625" style="40"/>
+    <col min="14593" max="14593" width="23.54296875" style="40" customWidth="1"/>
+    <col min="14594" max="14594" width="33.6328125" style="40" customWidth="1"/>
+    <col min="14595" max="14596" width="14.81640625" style="40" customWidth="1"/>
+    <col min="14597" max="14597" width="82.453125" style="40" customWidth="1"/>
+    <col min="14598" max="14848" width="14.81640625" style="40"/>
+    <col min="14849" max="14849" width="23.54296875" style="40" customWidth="1"/>
+    <col min="14850" max="14850" width="33.6328125" style="40" customWidth="1"/>
+    <col min="14851" max="14852" width="14.81640625" style="40" customWidth="1"/>
+    <col min="14853" max="14853" width="82.453125" style="40" customWidth="1"/>
+    <col min="14854" max="15104" width="14.81640625" style="40"/>
+    <col min="15105" max="15105" width="23.54296875" style="40" customWidth="1"/>
+    <col min="15106" max="15106" width="33.6328125" style="40" customWidth="1"/>
+    <col min="15107" max="15108" width="14.81640625" style="40" customWidth="1"/>
+    <col min="15109" max="15109" width="82.453125" style="40" customWidth="1"/>
+    <col min="15110" max="15360" width="14.81640625" style="40"/>
+    <col min="15361" max="15361" width="23.54296875" style="40" customWidth="1"/>
+    <col min="15362" max="15362" width="33.6328125" style="40" customWidth="1"/>
+    <col min="15363" max="15364" width="14.81640625" style="40" customWidth="1"/>
+    <col min="15365" max="15365" width="82.453125" style="40" customWidth="1"/>
+    <col min="15366" max="15616" width="14.81640625" style="40"/>
+    <col min="15617" max="15617" width="23.54296875" style="40" customWidth="1"/>
+    <col min="15618" max="15618" width="33.6328125" style="40" customWidth="1"/>
+    <col min="15619" max="15620" width="14.81640625" style="40" customWidth="1"/>
+    <col min="15621" max="15621" width="82.453125" style="40" customWidth="1"/>
+    <col min="15622" max="15872" width="14.81640625" style="40"/>
+    <col min="15873" max="15873" width="23.54296875" style="40" customWidth="1"/>
+    <col min="15874" max="15874" width="33.6328125" style="40" customWidth="1"/>
+    <col min="15875" max="15876" width="14.81640625" style="40" customWidth="1"/>
+    <col min="15877" max="15877" width="82.453125" style="40" customWidth="1"/>
+    <col min="15878" max="16128" width="14.81640625" style="40"/>
+    <col min="16129" max="16129" width="23.54296875" style="40" customWidth="1"/>
+    <col min="16130" max="16130" width="33.6328125" style="40" customWidth="1"/>
+    <col min="16131" max="16132" width="14.81640625" style="40" customWidth="1"/>
+    <col min="16133" max="16133" width="82.453125" style="40" customWidth="1"/>
+    <col min="16134" max="16384" width="14.81640625" style="40"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.399999999999999">
+    <row r="1" spans="1:5" ht="18">
       <c r="A1" s="76"/>
       <c r="B1" s="77"/>
       <c r="C1" s="77"/>
       <c r="D1" s="77"/>
       <c r="E1" s="77"/>
     </row>
-    <row r="2" spans="1:5" ht="14.4" thickBot="1">
+    <row r="2" spans="1:5" ht="14.5" thickBot="1">
       <c r="A2" s="77"/>
       <c r="B2" s="77"/>
       <c r="C2" s="77"/>
       <c r="D2" s="77"/>
       <c r="E2" s="77"/>
     </row>
-    <row r="3" spans="1:5" ht="13.95" customHeight="1">
+    <row r="3" spans="1:5" ht="14" customHeight="1">
       <c r="A3" s="160" t="s">
         <v>64</v>
       </c>
@@ -49073,14 +49038,14 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="14.4" thickBot="1">
+    <row r="4" spans="1:5" ht="14.5" thickBot="1">
       <c r="A4" s="161"/>
       <c r="B4" s="134"/>
       <c r="C4" s="134"/>
       <c r="D4" s="132"/>
       <c r="E4" s="134"/>
     </row>
-    <row r="5" spans="1:5" ht="13.95" customHeight="1">
+    <row r="5" spans="1:5" ht="14" customHeight="1">
       <c r="A5" s="153" t="s">
         <v>178</v>
       </c>
@@ -49134,7 +49099,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="13.95" customHeight="1">
+    <row r="9" spans="1:5" ht="14" customHeight="1">
       <c r="A9" s="137"/>
       <c r="B9" s="139"/>
       <c r="C9" s="79">
@@ -49292,7 +49257,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="14.4" thickBot="1">
+    <row r="21" spans="1:5" ht="14.5" thickBot="1">
       <c r="A21" s="138"/>
       <c r="B21" s="140"/>
       <c r="C21" s="81">
@@ -49305,7 +49270,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="13.95" customHeight="1">
+    <row r="22" spans="1:5" ht="14" customHeight="1">
       <c r="A22" s="141" t="s">
         <v>196</v>
       </c>
@@ -49385,7 +49350,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="14.4" thickBot="1">
+    <row r="28" spans="1:5" ht="14.5" thickBot="1">
       <c r="A28" s="142"/>
       <c r="B28" s="144"/>
       <c r="C28" s="80">
@@ -49621,7 +49586,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="14.4" thickBot="1">
+    <row r="46" spans="1:5" ht="14.5" thickBot="1">
       <c r="A46" s="148"/>
       <c r="B46" s="152"/>
       <c r="C46" s="81">
@@ -49727,7 +49692,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="14.4" thickBot="1">
+    <row r="54" spans="1:5" ht="14.5" thickBot="1">
       <c r="A54" s="94"/>
       <c r="B54" s="102"/>
       <c r="C54" s="81">
@@ -49774,15 +49739,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A5:E367"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView topLeftCell="A352" workbookViewId="0">
+      <selection activeCell="C363" sqref="C363"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="30.5546875" customWidth="1"/>
-    <col min="2" max="2" width="68.88671875" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="30.54296875" customWidth="1"/>
+    <col min="2" max="2" width="68.90625" customWidth="1"/>
+    <col min="3" max="3" width="20.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:5">
@@ -50015,7 +49980,7 @@
         <v>320</v>
       </c>
       <c r="C26" s="1">
-        <v>490546</v>
+        <v>794253</v>
       </c>
       <c r="D26" s="1">
         <v>1</v>
@@ -50270,7 +50235,7 @@
         <v>320</v>
       </c>
       <c r="C51" s="1">
-        <v>490546</v>
+        <v>794253</v>
       </c>
       <c r="D51" s="1">
         <v>1</v>
@@ -50536,7 +50501,7 @@
         <v>320</v>
       </c>
       <c r="C79" s="1">
-        <v>490546</v>
+        <v>794253</v>
       </c>
       <c r="D79" s="1">
         <v>1</v>
@@ -50824,7 +50789,7 @@
         <v>320</v>
       </c>
       <c r="C107" s="1">
-        <v>490546</v>
+        <v>794253</v>
       </c>
       <c r="D107" s="1">
         <v>1</v>
@@ -51090,7 +51055,7 @@
         <v>320</v>
       </c>
       <c r="C135" s="1">
-        <v>490546</v>
+        <v>794253</v>
       </c>
       <c r="D135" s="1">
         <v>1</v>
@@ -51356,7 +51321,7 @@
         <v>320</v>
       </c>
       <c r="C162" s="1">
-        <v>490546</v>
+        <v>794253</v>
       </c>
       <c r="D162" s="1">
         <v>1</v>
@@ -51622,7 +51587,7 @@
         <v>320</v>
       </c>
       <c r="C192" s="1">
-        <v>490546</v>
+        <v>794253</v>
       </c>
       <c r="D192" s="1">
         <v>1</v>
@@ -51888,7 +51853,7 @@
         <v>320</v>
       </c>
       <c r="C223" s="1">
-        <v>490546</v>
+        <v>794253</v>
       </c>
       <c r="D223" s="1">
         <v>1</v>
@@ -52165,7 +52130,7 @@
         <v>320</v>
       </c>
       <c r="C251" s="1">
-        <v>490546</v>
+        <v>794253</v>
       </c>
       <c r="D251" s="1">
         <v>1</v>
@@ -52431,7 +52396,7 @@
         <v>320</v>
       </c>
       <c r="C279" s="1">
-        <v>490546</v>
+        <v>794253</v>
       </c>
       <c r="D279" s="1">
         <v>1</v>
@@ -52697,7 +52662,7 @@
         <v>320</v>
       </c>
       <c r="C307" s="1">
-        <v>490546</v>
+        <v>794253</v>
       </c>
       <c r="D307" s="1">
         <v>1</v>
@@ -52963,7 +52928,7 @@
         <v>320</v>
       </c>
       <c r="C335" s="1">
-        <v>490546</v>
+        <v>794253</v>
       </c>
       <c r="D335" s="1">
         <v>1</v>
@@ -53229,7 +53194,7 @@
         <v>320</v>
       </c>
       <c r="C363" s="1">
-        <v>490546</v>
+        <v>794253</v>
       </c>
       <c r="D363" s="1">
         <v>1</v>
@@ -53293,10 +53258,10 @@
       <selection activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="3" max="3" width="28.33203125" customWidth="1"/>
-    <col min="4" max="4" width="79.21875" customWidth="1"/>
+    <col min="3" max="3" width="28.36328125" customWidth="1"/>
+    <col min="4" max="4" width="79.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="3:4">
@@ -54125,10 +54090,10 @@
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="4" max="4" width="21.6640625" customWidth="1"/>
-    <col min="5" max="5" width="84.88671875" customWidth="1"/>
+    <col min="4" max="4" width="21.6328125" customWidth="1"/>
+    <col min="5" max="5" width="84.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="4:5">
@@ -54433,11 +54398,11 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="69.44140625" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" customWidth="1"/>
+    <col min="2" max="2" width="69.453125" customWidth="1"/>
+    <col min="3" max="3" width="22.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:5">
@@ -57948,11 +57913,11 @@
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="27.5546875" customWidth="1"/>
-    <col min="2" max="2" width="68.44140625" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="1" max="1" width="27.54296875" customWidth="1"/>
+    <col min="2" max="2" width="68.453125" customWidth="1"/>
+    <col min="3" max="3" width="23.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:5">
@@ -61320,12 +61285,12 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.21875" customWidth="1"/>
-    <col min="2" max="2" width="67.44140625" customWidth="1"/>
-    <col min="3" max="3" width="22.77734375" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="23.1796875" customWidth="1"/>
+    <col min="2" max="2" width="67.453125" customWidth="1"/>
+    <col min="3" max="3" width="22.81640625" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:5">
@@ -64882,15 +64847,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A5:E367"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A352" workbookViewId="0">
+      <selection activeCell="B356" sqref="B356"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" customWidth="1"/>
-    <col min="2" max="2" width="68.88671875" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="26.90625" customWidth="1"/>
+    <col min="2" max="2" width="68.90625" customWidth="1"/>
+    <col min="3" max="3" width="20.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:5">
@@ -65123,7 +65088,7 @@
         <v>320</v>
       </c>
       <c r="C26" s="1">
-        <v>490546</v>
+        <v>794253</v>
       </c>
       <c r="D26" s="1">
         <v>1</v>
@@ -65378,7 +65343,7 @@
         <v>320</v>
       </c>
       <c r="C51" s="1">
-        <v>490546</v>
+        <v>794253</v>
       </c>
       <c r="D51" s="1">
         <v>1</v>
@@ -65644,7 +65609,7 @@
         <v>320</v>
       </c>
       <c r="C79" s="1">
-        <v>490546</v>
+        <v>794253</v>
       </c>
       <c r="D79" s="1">
         <v>1</v>
@@ -65932,7 +65897,7 @@
         <v>320</v>
       </c>
       <c r="C107" s="1">
-        <v>490546</v>
+        <v>794253</v>
       </c>
       <c r="D107" s="1">
         <v>1</v>
@@ -66198,7 +66163,7 @@
         <v>320</v>
       </c>
       <c r="C135" s="1">
-        <v>490546</v>
+        <v>794253</v>
       </c>
       <c r="D135" s="1">
         <v>1</v>
@@ -66464,7 +66429,7 @@
         <v>320</v>
       </c>
       <c r="C162" s="1">
-        <v>490546</v>
+        <v>794253</v>
       </c>
       <c r="D162" s="1">
         <v>1</v>
@@ -66730,7 +66695,7 @@
         <v>320</v>
       </c>
       <c r="C192" s="1">
-        <v>490546</v>
+        <v>794253</v>
       </c>
       <c r="D192" s="1">
         <v>1</v>
@@ -66996,7 +66961,7 @@
         <v>320</v>
       </c>
       <c r="C223" s="1">
-        <v>490546</v>
+        <v>794253</v>
       </c>
       <c r="D223" s="1">
         <v>1</v>
@@ -67273,7 +67238,7 @@
         <v>320</v>
       </c>
       <c r="C251" s="1">
-        <v>490546</v>
+        <v>794253</v>
       </c>
       <c r="D251" s="1">
         <v>1</v>
@@ -67539,7 +67504,7 @@
         <v>320</v>
       </c>
       <c r="C279" s="1">
-        <v>490546</v>
+        <v>794253</v>
       </c>
       <c r="D279" s="1">
         <v>1</v>
@@ -67805,7 +67770,7 @@
         <v>320</v>
       </c>
       <c r="C307" s="1">
-        <v>490546</v>
+        <v>794253</v>
       </c>
       <c r="D307" s="1">
         <v>1</v>
@@ -68071,7 +68036,7 @@
         <v>320</v>
       </c>
       <c r="C335" s="1">
-        <v>490546</v>
+        <v>794253</v>
       </c>
       <c r="D335" s="1">
         <v>1</v>
@@ -68337,7 +68302,7 @@
         <v>320</v>
       </c>
       <c r="C363" s="1">
-        <v>490546</v>
+        <v>794253</v>
       </c>
       <c r="D363" s="1">
         <v>1</v>
@@ -68401,11 +68366,11 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" customWidth="1"/>
-    <col min="2" max="2" width="69.44140625" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" customWidth="1"/>
+    <col min="1" max="1" width="25.36328125" customWidth="1"/>
+    <col min="2" max="2" width="69.453125" customWidth="1"/>
+    <col min="3" max="3" width="22.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:5">
@@ -71916,12 +71881,12 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="24.109375" customWidth="1"/>
-    <col min="2" max="2" width="68.44140625" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="24.08984375" customWidth="1"/>
+    <col min="2" max="2" width="68.453125" customWidth="1"/>
+    <col min="3" max="3" width="23.08984375" customWidth="1"/>
+    <col min="5" max="5" width="10.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:5">
@@ -75289,13 +75254,13 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="30.109375" customWidth="1"/>
-    <col min="2" max="2" width="67.44140625" customWidth="1"/>
-    <col min="3" max="3" width="22.77734375" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" customWidth="1"/>
-    <col min="5" max="5" width="13.77734375" customWidth="1"/>
+    <col min="1" max="1" width="30.08984375" customWidth="1"/>
+    <col min="2" max="2" width="67.453125" customWidth="1"/>
+    <col min="3" max="3" width="22.81640625" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" customWidth="1"/>
+    <col min="5" max="5" width="13.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:6">

</xml_diff>